<commit_message>
updated abstract excel file
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5C21E7-6805-6441-AB1C-B73819343AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DDE66A-A299-1548-8657-882992B87B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31100" yWindow="500" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="1300" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4265,7 +4265,7 @@
   <cols>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
continued changes to absract excel
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DDE66A-A299-1548-8657-882992B87B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242766F7-F589-5A41-B725-CD39C404E515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="1300" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44000" yWindow="820" windowWidth="24260" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="640">
   <si>
     <t>type</t>
   </si>
@@ -3881,6 +3881,207 @@
   <si>
     <t>notes</t>
   </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>includes figure, disclosures</t>
+  </si>
+  <si>
+    <t>original language but no language attribute</t>
+  </si>
+  <si>
+    <t>chemistry notation; MathML</t>
+  </si>
+  <si>
+    <t>includes table</t>
+  </si>
+  <si>
+    <t>table is wrapped in jats tags</t>
+  </si>
+  <si>
+    <t>includes both "ru" and "en" versions</t>
+  </si>
+  <si>
+    <t>lovely structured abstract</t>
+  </si>
+  <si>
+    <t>includes script from the landing page</t>
+  </si>
+  <si>
+    <t>includes links and script from the landing page that have been cut and paste into the abstract</t>
+  </si>
+  <si>
+    <t>includes figure, discosures; non-Latin char; MathML</t>
+  </si>
+  <si>
+    <t>has U+2008 General Punctuation non-Latin char; has journal level lang</t>
+  </si>
+  <si>
+    <t>non-Latin char; includes 3 languages in three &lt;jats:p&gt; elements</t>
+  </si>
+  <si>
+    <t>non-Latin char; includes disclosures</t>
+  </si>
+  <si>
+    <t>has U+2009 Thin Space General Punc char; lovely structured abstract</t>
+  </si>
+  <si>
+    <t>includes "ru", "key", "en" languages in metadata in that order, but no attributes; article in "ky" with "en" abstract, journal level is listed as "ru"</t>
+  </si>
+  <si>
+    <t>contains cyrillic char set; "ru","kz", "en",  languages in metadata in that order; should have had 3 abstracts each with their own language attribute</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>contains U+00A0 No Break Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MathML; </t>
+  </si>
+  <si>
+    <t>includes U+2771 Dingbat char</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-Latin char;  </t>
+  </si>
+  <si>
+    <t>includes links to png files but they are within the jats tags</t>
+  </si>
+  <si>
+    <t>article has "ru" and"en" versions</t>
+  </si>
+  <si>
+    <t>abstract does not render as full text for "ky" language; includes "ru", "ky","en" in that order</t>
+  </si>
+  <si>
+    <t>contains Latin-1 Supplement no break char</t>
+  </si>
+  <si>
+    <t>MathML; includes copyright statement</t>
+  </si>
+  <si>
+    <t>has &lt;jats: supplementary-material&gt; content</t>
+  </si>
+  <si>
+    <t>includes references</t>
+  </si>
+  <si>
+    <t>this is a medical abstract</t>
+  </si>
+  <si>
+    <t>includes U+200A Hair spaces, General Punctuation, includes hyperlinks</t>
+  </si>
+  <si>
+    <t>non-Latin char;  includes hyperlinnks</t>
+  </si>
+  <si>
+    <t>includes hyperlinks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes hyperlinks; includes funding acknowledgement; includes figures; </t>
+  </si>
+  <si>
+    <t>lovely structured abstract; poster abstract</t>
+  </si>
+  <si>
+    <t>XML_and_REST_agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes arabic, and latin char sets; Perfectly done with separate abstracts for each language and language attributes; the REST abstract only include "tr" while the XML response includes both "tr" and "en" versions. </t>
+  </si>
+  <si>
+    <t>"uk" and "en" included in the same abstract metadata element; latin and cyrillinc; language attribute was only "en"</t>
+  </si>
+  <si>
+    <t>"en"</t>
+  </si>
+  <si>
+    <t>"tr","en"</t>
+  </si>
+  <si>
+    <t>includes disclosures</t>
+  </si>
+  <si>
+    <t>includes 2 languages</t>
+  </si>
+  <si>
+    <t>includes 2 languages; non-Latin char</t>
+  </si>
+  <si>
+    <t>includes 2 languages; "ru" assigned to journal level but missing in abstract</t>
+  </si>
+  <si>
+    <t>"ru" and "en" included in the same abstract metadata element; latin and cyrillinc;</t>
+  </si>
+  <si>
+    <t>includes jats tagged bulleted list</t>
+  </si>
+  <si>
+    <t>U+2008 punctuation space from general punc</t>
+  </si>
+  <si>
+    <t>non-Latin char;  includes figure; includes disclosures</t>
+  </si>
+  <si>
+    <t>all in same element; includes U+200A Hair spaces; includes keywords</t>
+  </si>
+  <si>
+    <t>includes 3 languages; non-Latin char</t>
+  </si>
+  <si>
+    <t>"en", "kz", "ru" in article and same metadata element; Latin and Cyrillic char sets</t>
+  </si>
+  <si>
+    <t>includes full citation format in the abstract</t>
+  </si>
+  <si>
+    <t>medical abstract</t>
+  </si>
+  <si>
+    <t>poster abstract</t>
+  </si>
+  <si>
+    <t>includes figure, acknowledgements</t>
+  </si>
+  <si>
+    <t>non-Latin char; includes disclosures; includes figure</t>
+  </si>
+  <si>
+    <t>U+2009 thin space from general punc; lovely structured abstract</t>
+  </si>
+  <si>
+    <t>U+2008 punctuation space from general punc; lovely structured abstract</t>
+  </si>
+  <si>
+    <t>U+2009 thin space from general punc; whole medical abstract</t>
+  </si>
+  <si>
+    <t>No problems</t>
+  </si>
+  <si>
+    <t>no problems, marked correctly as retracted in metadata</t>
+  </si>
+  <si>
+    <t>marked as retracted</t>
+  </si>
+  <si>
+    <t>U+200a hair space and U+2009 thin space</t>
+  </si>
+  <si>
+    <t>non-Latin char; includes hyperlinks</t>
+  </si>
+  <si>
+    <t>front matter; includes personal contact information</t>
+  </si>
+  <si>
+    <t>includes funding acknowledgement</t>
+  </si>
 </sst>
 </file>
 
@@ -3901,12 +4102,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -3945,14 +4152,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4255,26 +4469,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L301"/>
+  <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.33203125" customWidth="1"/>
+    <col min="4" max="4" width="135.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="42.1640625" customWidth="1"/>
+    <col min="13" max="13" width="75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4303,13 +4521,16 @@
         <v>571</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4319,14 +4540,35 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E2">
         <v>10871</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>573</v>
+      </c>
+      <c r="G2" t="s">
+        <v>574</v>
+      </c>
+      <c r="H2" t="s">
+        <v>573</v>
+      </c>
+      <c r="I2" t="s">
+        <v>573</v>
+      </c>
+      <c r="J2" t="s">
+        <v>574</v>
+      </c>
+      <c r="K2" t="s">
+        <v>573</v>
+      </c>
+      <c r="L2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4336,14 +4578,35 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3">
         <v>10055</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>573</v>
+      </c>
+      <c r="G3" t="s">
+        <v>574</v>
+      </c>
+      <c r="H3" t="s">
+        <v>573</v>
+      </c>
+      <c r="I3" t="s">
+        <v>573</v>
+      </c>
+      <c r="J3" t="s">
+        <v>574</v>
+      </c>
+      <c r="K3" t="s">
+        <v>573</v>
+      </c>
+      <c r="L3" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4359,8 +4622,29 @@
       <c r="E4">
         <v>9074</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>574</v>
+      </c>
+      <c r="G4" t="s">
+        <v>574</v>
+      </c>
+      <c r="H4" t="s">
+        <v>573</v>
+      </c>
+      <c r="I4" t="s">
+        <v>573</v>
+      </c>
+      <c r="J4" t="s">
+        <v>574</v>
+      </c>
+      <c r="K4" t="s">
+        <v>573</v>
+      </c>
+      <c r="L4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4376,8 +4660,32 @@
       <c r="E5">
         <v>7376</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>574</v>
+      </c>
+      <c r="G5" t="s">
+        <v>574</v>
+      </c>
+      <c r="H5" t="s">
+        <v>573</v>
+      </c>
+      <c r="I5" t="s">
+        <v>573</v>
+      </c>
+      <c r="J5" t="s">
+        <v>574</v>
+      </c>
+      <c r="K5" t="s">
+        <v>573</v>
+      </c>
+      <c r="L5" t="s">
+        <v>578</v>
+      </c>
+      <c r="M5" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4393,8 +4701,32 @@
       <c r="E6">
         <v>7351</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>574</v>
+      </c>
+      <c r="G6" t="s">
+        <v>574</v>
+      </c>
+      <c r="H6" t="s">
+        <v>573</v>
+      </c>
+      <c r="I6" t="s">
+        <v>573</v>
+      </c>
+      <c r="J6" t="s">
+        <v>574</v>
+      </c>
+      <c r="K6" t="s">
+        <v>573</v>
+      </c>
+      <c r="L6" t="s">
+        <v>617</v>
+      </c>
+      <c r="M6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4410,8 +4742,29 @@
       <c r="E7">
         <v>7320</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>574</v>
+      </c>
+      <c r="G7" t="s">
+        <v>574</v>
+      </c>
+      <c r="H7" t="s">
+        <v>573</v>
+      </c>
+      <c r="I7" t="s">
+        <v>573</v>
+      </c>
+      <c r="J7" t="s">
+        <v>574</v>
+      </c>
+      <c r="K7" t="s">
+        <v>573</v>
+      </c>
+      <c r="L7" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4427,8 +4780,32 @@
       <c r="E8">
         <v>7077</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>574</v>
+      </c>
+      <c r="G8" t="s">
+        <v>574</v>
+      </c>
+      <c r="H8" t="s">
+        <v>573</v>
+      </c>
+      <c r="I8" t="s">
+        <v>573</v>
+      </c>
+      <c r="J8" t="s">
+        <v>574</v>
+      </c>
+      <c r="K8" t="s">
+        <v>573</v>
+      </c>
+      <c r="L8" t="s">
+        <v>633</v>
+      </c>
+      <c r="M8" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4444,8 +4821,32 @@
       <c r="E9">
         <v>6937</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>573</v>
+      </c>
+      <c r="G9" t="s">
+        <v>574</v>
+      </c>
+      <c r="H9" t="s">
+        <v>574</v>
+      </c>
+      <c r="I9" t="s">
+        <v>574</v>
+      </c>
+      <c r="J9" t="s">
+        <v>574</v>
+      </c>
+      <c r="K9" t="s">
+        <v>573</v>
+      </c>
+      <c r="L9" t="s">
+        <v>582</v>
+      </c>
+      <c r="M9" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4461,8 +4862,29 @@
       <c r="E10">
         <v>6602</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>573</v>
+      </c>
+      <c r="G10" t="s">
+        <v>573</v>
+      </c>
+      <c r="H10" t="s">
+        <v>573</v>
+      </c>
+      <c r="I10" t="s">
+        <v>573</v>
+      </c>
+      <c r="J10" t="s">
+        <v>574</v>
+      </c>
+      <c r="K10" t="s">
+        <v>573</v>
+      </c>
+      <c r="L10" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4478,8 +4900,32 @@
       <c r="E11">
         <v>6576</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>573</v>
+      </c>
+      <c r="G11" t="s">
+        <v>574</v>
+      </c>
+      <c r="H11" t="s">
+        <v>573</v>
+      </c>
+      <c r="I11" t="s">
+        <v>573</v>
+      </c>
+      <c r="J11" t="s">
+        <v>574</v>
+      </c>
+      <c r="K11" t="s">
+        <v>573</v>
+      </c>
+      <c r="L11" t="s">
+        <v>584</v>
+      </c>
+      <c r="M11" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4495,8 +4941,32 @@
       <c r="E12">
         <v>6561</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>574</v>
+      </c>
+      <c r="G12" t="s">
+        <v>574</v>
+      </c>
+      <c r="H12" t="s">
+        <v>573</v>
+      </c>
+      <c r="I12" t="s">
+        <v>573</v>
+      </c>
+      <c r="J12" t="s">
+        <v>574</v>
+      </c>
+      <c r="K12" t="s">
+        <v>573</v>
+      </c>
+      <c r="L12" t="s">
+        <v>586</v>
+      </c>
+      <c r="M12" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4512,8 +4982,32 @@
       <c r="E13">
         <v>6536</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>574</v>
+      </c>
+      <c r="G13" t="s">
+        <v>574</v>
+      </c>
+      <c r="H13" t="s">
+        <v>573</v>
+      </c>
+      <c r="I13" t="s">
+        <v>573</v>
+      </c>
+      <c r="J13" t="s">
+        <v>574</v>
+      </c>
+      <c r="K13" t="s">
+        <v>573</v>
+      </c>
+      <c r="L13" t="s">
+        <v>587</v>
+      </c>
+      <c r="M13" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4529,8 +5023,32 @@
       <c r="E14">
         <v>6391</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>574</v>
+      </c>
+      <c r="G14" t="s">
+        <v>574</v>
+      </c>
+      <c r="H14" t="s">
+        <v>591</v>
+      </c>
+      <c r="I14" t="s">
+        <v>574</v>
+      </c>
+      <c r="J14" t="s">
+        <v>574</v>
+      </c>
+      <c r="K14" t="s">
+        <v>573</v>
+      </c>
+      <c r="L14" t="s">
+        <v>586</v>
+      </c>
+      <c r="M14" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4546,8 +5064,29 @@
       <c r="E15">
         <v>5880</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>574</v>
+      </c>
+      <c r="G15" t="s">
+        <v>574</v>
+      </c>
+      <c r="H15" t="s">
+        <v>573</v>
+      </c>
+      <c r="I15" t="s">
+        <v>573</v>
+      </c>
+      <c r="J15" t="s">
+        <v>574</v>
+      </c>
+      <c r="K15" t="s">
+        <v>573</v>
+      </c>
+      <c r="L15" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4563,8 +5102,32 @@
       <c r="E16">
         <v>5878</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>573</v>
+      </c>
+      <c r="G16" t="s">
+        <v>574</v>
+      </c>
+      <c r="H16" t="s">
+        <v>573</v>
+      </c>
+      <c r="I16" t="s">
+        <v>573</v>
+      </c>
+      <c r="J16" t="s">
+        <v>574</v>
+      </c>
+      <c r="K16" t="s">
+        <v>573</v>
+      </c>
+      <c r="L16" t="s">
+        <v>593</v>
+      </c>
+      <c r="M16" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4580,8 +5143,32 @@
       <c r="E17">
         <v>5605</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>574</v>
+      </c>
+      <c r="G17" t="s">
+        <v>574</v>
+      </c>
+      <c r="H17" t="s">
+        <v>573</v>
+      </c>
+      <c r="I17" t="s">
+        <v>573</v>
+      </c>
+      <c r="J17" t="s">
+        <v>574</v>
+      </c>
+      <c r="K17" t="s">
+        <v>573</v>
+      </c>
+      <c r="L17" t="s">
+        <v>595</v>
+      </c>
+      <c r="M17" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4597,8 +5184,32 @@
       <c r="E18">
         <v>5526</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>573</v>
+      </c>
+      <c r="G18" t="s">
+        <v>574</v>
+      </c>
+      <c r="H18" t="s">
+        <v>573</v>
+      </c>
+      <c r="I18" t="s">
+        <v>573</v>
+      </c>
+      <c r="J18" t="s">
+        <v>574</v>
+      </c>
+      <c r="K18" t="s">
+        <v>573</v>
+      </c>
+      <c r="L18" t="s">
+        <v>606</v>
+      </c>
+      <c r="M18" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4614,8 +5225,32 @@
       <c r="E19">
         <v>5501</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>574</v>
+      </c>
+      <c r="G19" t="s">
+        <v>574</v>
+      </c>
+      <c r="H19" t="s">
+        <v>574</v>
+      </c>
+      <c r="I19" t="s">
+        <v>573</v>
+      </c>
+      <c r="J19" t="s">
+        <v>574</v>
+      </c>
+      <c r="K19" t="s">
+        <v>573</v>
+      </c>
+      <c r="L19" t="s">
+        <v>615</v>
+      </c>
+      <c r="M19" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4631,8 +5266,29 @@
       <c r="E20">
         <v>5490</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>573</v>
+      </c>
+      <c r="G20" t="s">
+        <v>574</v>
+      </c>
+      <c r="H20" t="s">
+        <v>573</v>
+      </c>
+      <c r="I20" t="s">
+        <v>573</v>
+      </c>
+      <c r="J20" t="s">
+        <v>574</v>
+      </c>
+      <c r="K20" t="s">
+        <v>573</v>
+      </c>
+      <c r="L20" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4642,14 +5298,38 @@
       <c r="C21" t="s">
         <v>43</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E21">
         <v>5421</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>574</v>
+      </c>
+      <c r="G21" t="s">
+        <v>574</v>
+      </c>
+      <c r="H21" t="s">
+        <v>591</v>
+      </c>
+      <c r="I21" t="s">
+        <v>573</v>
+      </c>
+      <c r="J21" t="s">
+        <v>574</v>
+      </c>
+      <c r="K21" t="s">
+        <v>573</v>
+      </c>
+      <c r="L21" t="s">
+        <v>586</v>
+      </c>
+      <c r="M21" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4665,8 +5345,32 @@
       <c r="E22">
         <v>5297</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>574</v>
+      </c>
+      <c r="G22" t="s">
+        <v>574</v>
+      </c>
+      <c r="H22" t="s">
+        <v>573</v>
+      </c>
+      <c r="I22" t="s">
+        <v>573</v>
+      </c>
+      <c r="J22" t="s">
+        <v>574</v>
+      </c>
+      <c r="K22" t="s">
+        <v>573</v>
+      </c>
+      <c r="L22" t="s">
+        <v>595</v>
+      </c>
+      <c r="M22" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4682,8 +5386,32 @@
       <c r="E23">
         <v>5272</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>573</v>
+      </c>
+      <c r="G23" t="s">
+        <v>574</v>
+      </c>
+      <c r="H23" t="s">
+        <v>573</v>
+      </c>
+      <c r="I23" t="s">
+        <v>573</v>
+      </c>
+      <c r="J23" t="s">
+        <v>574</v>
+      </c>
+      <c r="K23" t="s">
+        <v>573</v>
+      </c>
+      <c r="L23" t="s">
+        <v>593</v>
+      </c>
+      <c r="M23" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4699,8 +5427,32 @@
       <c r="E24">
         <v>5209</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>573</v>
+      </c>
+      <c r="G24" t="s">
+        <v>574</v>
+      </c>
+      <c r="H24" t="s">
+        <v>573</v>
+      </c>
+      <c r="I24" t="s">
+        <v>573</v>
+      </c>
+      <c r="J24" t="s">
+        <v>574</v>
+      </c>
+      <c r="K24" t="s">
+        <v>573</v>
+      </c>
+      <c r="L24" t="s">
+        <v>600</v>
+      </c>
+      <c r="M24" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4716,8 +5468,32 @@
       <c r="E25">
         <v>5186</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>574</v>
+      </c>
+      <c r="G25" t="s">
+        <v>612</v>
+      </c>
+      <c r="H25" t="s">
+        <v>573</v>
+      </c>
+      <c r="I25" t="s">
+        <v>573</v>
+      </c>
+      <c r="J25" t="s">
+        <v>574</v>
+      </c>
+      <c r="K25" t="s">
+        <v>573</v>
+      </c>
+      <c r="L25" t="s">
+        <v>633</v>
+      </c>
+      <c r="M25" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4733,8 +5509,32 @@
       <c r="E26">
         <v>5162</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>573</v>
+      </c>
+      <c r="G26" t="s">
+        <v>574</v>
+      </c>
+      <c r="H26" t="s">
+        <v>573</v>
+      </c>
+      <c r="I26" t="s">
+        <v>573</v>
+      </c>
+      <c r="J26" t="s">
+        <v>574</v>
+      </c>
+      <c r="K26" t="s">
+        <v>573</v>
+      </c>
+      <c r="L26" t="s">
+        <v>593</v>
+      </c>
+      <c r="M26" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4750,8 +5550,29 @@
       <c r="E27">
         <v>5140</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>574</v>
+      </c>
+      <c r="G27" t="s">
+        <v>612</v>
+      </c>
+      <c r="H27" t="s">
+        <v>573</v>
+      </c>
+      <c r="I27" t="s">
+        <v>573</v>
+      </c>
+      <c r="J27" t="s">
+        <v>574</v>
+      </c>
+      <c r="K27" t="s">
+        <v>573</v>
+      </c>
+      <c r="L27" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4767,8 +5588,32 @@
       <c r="E28">
         <v>5103</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>574</v>
+      </c>
+      <c r="G28" t="s">
+        <v>574</v>
+      </c>
+      <c r="H28" t="s">
+        <v>573</v>
+      </c>
+      <c r="I28" t="s">
+        <v>573</v>
+      </c>
+      <c r="J28" t="s">
+        <v>574</v>
+      </c>
+      <c r="K28" t="s">
+        <v>573</v>
+      </c>
+      <c r="L28" t="s">
+        <v>602</v>
+      </c>
+      <c r="M28" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4784,8 +5629,32 @@
       <c r="E29">
         <v>5091</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>574</v>
+      </c>
+      <c r="G29" t="s">
+        <v>574</v>
+      </c>
+      <c r="H29" t="s">
+        <v>573</v>
+      </c>
+      <c r="I29" t="s">
+        <v>573</v>
+      </c>
+      <c r="J29" t="s">
+        <v>574</v>
+      </c>
+      <c r="K29" t="s">
+        <v>573</v>
+      </c>
+      <c r="L29" t="s">
+        <v>605</v>
+      </c>
+      <c r="M29" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4801,8 +5670,29 @@
       <c r="E30">
         <v>5038</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>574</v>
+      </c>
+      <c r="G30" t="s">
+        <v>574</v>
+      </c>
+      <c r="H30" t="s">
+        <v>573</v>
+      </c>
+      <c r="I30" t="s">
+        <v>591</v>
+      </c>
+      <c r="J30" t="s">
+        <v>574</v>
+      </c>
+      <c r="K30" t="s">
+        <v>573</v>
+      </c>
+      <c r="L30" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4818,25 +5708,73 @@
       <c r="E31">
         <v>4912</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="F31" t="s">
+        <v>574</v>
+      </c>
+      <c r="G31" t="s">
+        <v>574</v>
+      </c>
+      <c r="H31" t="s">
+        <v>573</v>
+      </c>
+      <c r="I31" t="s">
+        <v>573</v>
+      </c>
+      <c r="J31" t="s">
+        <v>574</v>
+      </c>
+      <c r="K31" t="s">
+        <v>573</v>
+      </c>
+      <c r="L31" t="s">
+        <v>633</v>
+      </c>
+      <c r="M31" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="5">
         <v>4899</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4852,8 +5790,32 @@
       <c r="E33">
         <v>4899</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>574</v>
+      </c>
+      <c r="G33" t="s">
+        <v>612</v>
+      </c>
+      <c r="H33" t="s">
+        <v>574</v>
+      </c>
+      <c r="I33" t="s">
+        <v>573</v>
+      </c>
+      <c r="J33" t="s">
+        <v>574</v>
+      </c>
+      <c r="K33" t="s">
+        <v>573</v>
+      </c>
+      <c r="L33" t="s">
+        <v>616</v>
+      </c>
+      <c r="M33" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4869,8 +5831,29 @@
       <c r="E34">
         <v>4893</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>574</v>
+      </c>
+      <c r="G34" t="s">
+        <v>574</v>
+      </c>
+      <c r="H34" t="s">
+        <v>573</v>
+      </c>
+      <c r="I34" t="s">
+        <v>591</v>
+      </c>
+      <c r="J34" t="s">
+        <v>574</v>
+      </c>
+      <c r="K34" t="s">
+        <v>573</v>
+      </c>
+      <c r="L34" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4886,8 +5869,32 @@
       <c r="E35">
         <v>4889</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>574</v>
+      </c>
+      <c r="G35" t="s">
+        <v>574</v>
+      </c>
+      <c r="H35" t="s">
+        <v>573</v>
+      </c>
+      <c r="I35" t="s">
+        <v>591</v>
+      </c>
+      <c r="J35" t="s">
+        <v>574</v>
+      </c>
+      <c r="K35" t="s">
+        <v>573</v>
+      </c>
+      <c r="L35" t="s">
+        <v>616</v>
+      </c>
+      <c r="M35" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4903,8 +5910,32 @@
       <c r="E36">
         <v>4842</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>574</v>
+      </c>
+      <c r="G36" t="s">
+        <v>574</v>
+      </c>
+      <c r="H36" t="s">
+        <v>591</v>
+      </c>
+      <c r="I36" t="s">
+        <v>573</v>
+      </c>
+      <c r="J36" t="s">
+        <v>574</v>
+      </c>
+      <c r="K36" t="s">
+        <v>573</v>
+      </c>
+      <c r="L36" t="s">
+        <v>616</v>
+      </c>
+      <c r="M36" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4920,8 +5951,32 @@
       <c r="E37">
         <v>4836</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>574</v>
+      </c>
+      <c r="G37" t="s">
+        <v>574</v>
+      </c>
+      <c r="H37" t="s">
+        <v>591</v>
+      </c>
+      <c r="I37" t="s">
+        <v>573</v>
+      </c>
+      <c r="J37" t="s">
+        <v>574</v>
+      </c>
+      <c r="K37" t="s">
+        <v>573</v>
+      </c>
+      <c r="L37" t="s">
+        <v>616</v>
+      </c>
+      <c r="M37" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4937,8 +5992,29 @@
       <c r="E38">
         <v>4833</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>574</v>
+      </c>
+      <c r="G38" t="s">
+        <v>574</v>
+      </c>
+      <c r="H38" t="s">
+        <v>573</v>
+      </c>
+      <c r="I38" t="s">
+        <v>573</v>
+      </c>
+      <c r="J38" t="s">
+        <v>574</v>
+      </c>
+      <c r="K38" t="s">
+        <v>573</v>
+      </c>
+      <c r="L38" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4954,8 +6030,32 @@
       <c r="E39">
         <v>4815</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>574</v>
+      </c>
+      <c r="G39" t="s">
+        <v>612</v>
+      </c>
+      <c r="H39" t="s">
+        <v>573</v>
+      </c>
+      <c r="I39" t="s">
+        <v>573</v>
+      </c>
+      <c r="J39" t="s">
+        <v>574</v>
+      </c>
+      <c r="K39" t="s">
+        <v>573</v>
+      </c>
+      <c r="L39" t="s">
+        <v>633</v>
+      </c>
+      <c r="M39" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4971,8 +6071,32 @@
       <c r="E40">
         <v>4815</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>574</v>
+      </c>
+      <c r="G40" t="s">
+        <v>574</v>
+      </c>
+      <c r="H40" t="s">
+        <v>573</v>
+      </c>
+      <c r="I40" t="s">
+        <v>591</v>
+      </c>
+      <c r="J40" t="s">
+        <v>574</v>
+      </c>
+      <c r="K40" t="s">
+        <v>573</v>
+      </c>
+      <c r="L40" t="s">
+        <v>621</v>
+      </c>
+      <c r="M40" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4988,8 +6112,32 @@
       <c r="E41">
         <v>4809</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>574</v>
+      </c>
+      <c r="G41" t="s">
+        <v>574</v>
+      </c>
+      <c r="H41" t="s">
+        <v>573</v>
+      </c>
+      <c r="I41" t="s">
+        <v>573</v>
+      </c>
+      <c r="J41" t="s">
+        <v>574</v>
+      </c>
+      <c r="K41" t="s">
+        <v>573</v>
+      </c>
+      <c r="L41" t="s">
+        <v>616</v>
+      </c>
+      <c r="M41" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -5005,8 +6153,32 @@
       <c r="E42">
         <v>4800</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>574</v>
+      </c>
+      <c r="G42" t="s">
+        <v>574</v>
+      </c>
+      <c r="H42" t="s">
+        <v>591</v>
+      </c>
+      <c r="I42" t="s">
+        <v>573</v>
+      </c>
+      <c r="J42" t="s">
+        <v>574</v>
+      </c>
+      <c r="K42" t="s">
+        <v>573</v>
+      </c>
+      <c r="L42" t="s">
+        <v>623</v>
+      </c>
+      <c r="M42" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -5022,8 +6194,29 @@
       <c r="E43">
         <v>4782</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>574</v>
+      </c>
+      <c r="G43" t="s">
+        <v>574</v>
+      </c>
+      <c r="H43" t="s">
+        <v>573</v>
+      </c>
+      <c r="I43" t="s">
+        <v>573</v>
+      </c>
+      <c r="J43" t="s">
+        <v>574</v>
+      </c>
+      <c r="K43" t="s">
+        <v>573</v>
+      </c>
+      <c r="L43" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -5039,8 +6232,29 @@
       <c r="E44">
         <v>4732</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>574</v>
+      </c>
+      <c r="G44" t="s">
+        <v>574</v>
+      </c>
+      <c r="H44" t="s">
+        <v>573</v>
+      </c>
+      <c r="I44" t="s">
+        <v>573</v>
+      </c>
+      <c r="J44" t="s">
+        <v>574</v>
+      </c>
+      <c r="K44" t="s">
+        <v>573</v>
+      </c>
+      <c r="L44" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -5056,8 +6270,32 @@
       <c r="E45">
         <v>4723</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>574</v>
+      </c>
+      <c r="G45" t="s">
+        <v>574</v>
+      </c>
+      <c r="H45" t="s">
+        <v>591</v>
+      </c>
+      <c r="I45" t="s">
+        <v>573</v>
+      </c>
+      <c r="J45" t="s">
+        <v>574</v>
+      </c>
+      <c r="K45" t="s">
+        <v>573</v>
+      </c>
+      <c r="L45" t="s">
+        <v>616</v>
+      </c>
+      <c r="M45" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5073,8 +6311,29 @@
       <c r="E46">
         <v>4719</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>574</v>
+      </c>
+      <c r="G46" t="s">
+        <v>574</v>
+      </c>
+      <c r="H46" t="s">
+        <v>573</v>
+      </c>
+      <c r="I46" t="s">
+        <v>591</v>
+      </c>
+      <c r="J46" t="s">
+        <v>574</v>
+      </c>
+      <c r="K46" t="s">
+        <v>573</v>
+      </c>
+      <c r="L46" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5090,8 +6349,32 @@
       <c r="E47">
         <v>4652</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>574</v>
+      </c>
+      <c r="G47" t="s">
+        <v>574</v>
+      </c>
+      <c r="H47" t="s">
+        <v>573</v>
+      </c>
+      <c r="I47" t="s">
+        <v>591</v>
+      </c>
+      <c r="J47" t="s">
+        <v>574</v>
+      </c>
+      <c r="K47" t="s">
+        <v>573</v>
+      </c>
+      <c r="L47" t="s">
+        <v>633</v>
+      </c>
+      <c r="M47" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -5107,8 +6390,32 @@
       <c r="E48">
         <v>4651</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>574</v>
+      </c>
+      <c r="G48" t="s">
+        <v>574</v>
+      </c>
+      <c r="H48" t="s">
+        <v>573</v>
+      </c>
+      <c r="I48" t="s">
+        <v>573</v>
+      </c>
+      <c r="J48" t="s">
+        <v>574</v>
+      </c>
+      <c r="K48" t="s">
+        <v>573</v>
+      </c>
+      <c r="L48" t="s">
+        <v>633</v>
+      </c>
+      <c r="M48" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -5124,8 +6431,32 @@
       <c r="E49">
         <v>4628</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>574</v>
+      </c>
+      <c r="G49" t="s">
+        <v>574</v>
+      </c>
+      <c r="H49" t="s">
+        <v>573</v>
+      </c>
+      <c r="I49" t="s">
+        <v>573</v>
+      </c>
+      <c r="J49" t="s">
+        <v>574</v>
+      </c>
+      <c r="K49" t="s">
+        <v>573</v>
+      </c>
+      <c r="L49" t="s">
+        <v>633</v>
+      </c>
+      <c r="M49" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -5141,8 +6472,32 @@
       <c r="E50">
         <v>4598</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>574</v>
+      </c>
+      <c r="G50" t="s">
+        <v>574</v>
+      </c>
+      <c r="H50" t="s">
+        <v>573</v>
+      </c>
+      <c r="I50" t="s">
+        <v>573</v>
+      </c>
+      <c r="J50" t="s">
+        <v>574</v>
+      </c>
+      <c r="K50" t="s">
+        <v>573</v>
+      </c>
+      <c r="L50" t="s">
+        <v>633</v>
+      </c>
+      <c r="M50" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -5158,8 +6513,29 @@
       <c r="E51">
         <v>4596</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>574</v>
+      </c>
+      <c r="G51" t="s">
+        <v>574</v>
+      </c>
+      <c r="H51" t="s">
+        <v>573</v>
+      </c>
+      <c r="I51" t="s">
+        <v>573</v>
+      </c>
+      <c r="J51" t="s">
+        <v>574</v>
+      </c>
+      <c r="K51" t="s">
+        <v>573</v>
+      </c>
+      <c r="L51" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -5175,8 +6551,32 @@
       <c r="E52">
         <v>4594</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>574</v>
+      </c>
+      <c r="G52" t="s">
+        <v>574</v>
+      </c>
+      <c r="H52" t="s">
+        <v>573</v>
+      </c>
+      <c r="I52" t="s">
+        <v>591</v>
+      </c>
+      <c r="J52" t="s">
+        <v>574</v>
+      </c>
+      <c r="K52" t="s">
+        <v>573</v>
+      </c>
+      <c r="L52" t="s">
+        <v>628</v>
+      </c>
+      <c r="M52" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -5192,8 +6592,32 @@
       <c r="E53">
         <v>4574</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>574</v>
+      </c>
+      <c r="G53" t="s">
+        <v>574</v>
+      </c>
+      <c r="H53" t="s">
+        <v>573</v>
+      </c>
+      <c r="I53" t="s">
+        <v>591</v>
+      </c>
+      <c r="J53" t="s">
+        <v>574</v>
+      </c>
+      <c r="K53" t="s">
+        <v>573</v>
+      </c>
+      <c r="L53" t="s">
+        <v>629</v>
+      </c>
+      <c r="M53" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -5209,8 +6633,32 @@
       <c r="E54">
         <v>4572</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>574</v>
+      </c>
+      <c r="G54" t="s">
+        <v>574</v>
+      </c>
+      <c r="H54" t="s">
+        <v>573</v>
+      </c>
+      <c r="I54" t="s">
+        <v>591</v>
+      </c>
+      <c r="J54" t="s">
+        <v>574</v>
+      </c>
+      <c r="K54" t="s">
+        <v>573</v>
+      </c>
+      <c r="L54" t="s">
+        <v>629</v>
+      </c>
+      <c r="M54" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -5226,8 +6674,32 @@
       <c r="E55">
         <v>4562</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>574</v>
+      </c>
+      <c r="G55" t="s">
+        <v>574</v>
+      </c>
+      <c r="H55" t="s">
+        <v>573</v>
+      </c>
+      <c r="I55" t="s">
+        <v>573</v>
+      </c>
+      <c r="J55" t="s">
+        <v>574</v>
+      </c>
+      <c r="K55" t="s">
+        <v>573</v>
+      </c>
+      <c r="L55" t="s">
+        <v>595</v>
+      </c>
+      <c r="M55" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -5243,8 +6715,32 @@
       <c r="E56">
         <v>4545</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>574</v>
+      </c>
+      <c r="G56" t="s">
+        <v>574</v>
+      </c>
+      <c r="H56" t="s">
+        <v>573</v>
+      </c>
+      <c r="I56" t="s">
+        <v>573</v>
+      </c>
+      <c r="J56" t="s">
+        <v>574</v>
+      </c>
+      <c r="K56" t="s">
+        <v>573</v>
+      </c>
+      <c r="L56" t="s">
+        <v>595</v>
+      </c>
+      <c r="M56" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -5260,8 +6756,32 @@
       <c r="E57">
         <v>4542</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>574</v>
+      </c>
+      <c r="G57" t="s">
+        <v>574</v>
+      </c>
+      <c r="H57" t="s">
+        <v>573</v>
+      </c>
+      <c r="I57" t="s">
+        <v>591</v>
+      </c>
+      <c r="J57" t="s">
+        <v>574</v>
+      </c>
+      <c r="K57" t="s">
+        <v>573</v>
+      </c>
+      <c r="L57" t="s">
+        <v>616</v>
+      </c>
+      <c r="M57" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5277,8 +6797,29 @@
       <c r="E58">
         <v>4540</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>574</v>
+      </c>
+      <c r="G58" t="s">
+        <v>574</v>
+      </c>
+      <c r="H58" t="s">
+        <v>573</v>
+      </c>
+      <c r="I58" t="s">
+        <v>573</v>
+      </c>
+      <c r="J58" t="s">
+        <v>574</v>
+      </c>
+      <c r="K58" t="s">
+        <v>573</v>
+      </c>
+      <c r="L58" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5294,8 +6835,29 @@
       <c r="E59">
         <v>4530</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>574</v>
+      </c>
+      <c r="G59" t="s">
+        <v>574</v>
+      </c>
+      <c r="H59" t="s">
+        <v>573</v>
+      </c>
+      <c r="I59" t="s">
+        <v>573</v>
+      </c>
+      <c r="J59" t="s">
+        <v>574</v>
+      </c>
+      <c r="K59" t="s">
+        <v>573</v>
+      </c>
+      <c r="L59" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5311,8 +6873,32 @@
       <c r="E60">
         <v>4483</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>574</v>
+      </c>
+      <c r="G60" t="s">
+        <v>574</v>
+      </c>
+      <c r="H60" t="s">
+        <v>573</v>
+      </c>
+      <c r="I60" t="s">
+        <v>591</v>
+      </c>
+      <c r="J60" t="s">
+        <v>574</v>
+      </c>
+      <c r="K60" t="s">
+        <v>573</v>
+      </c>
+      <c r="L60" t="s">
+        <v>635</v>
+      </c>
+      <c r="M60" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5328,8 +6914,32 @@
       <c r="E61">
         <v>4419</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>574</v>
+      </c>
+      <c r="G61" t="s">
+        <v>574</v>
+      </c>
+      <c r="H61" t="s">
+        <v>573</v>
+      </c>
+      <c r="I61" t="s">
+        <v>574</v>
+      </c>
+      <c r="J61" t="s">
+        <v>574</v>
+      </c>
+      <c r="K61" t="s">
+        <v>573</v>
+      </c>
+      <c r="L61" t="s">
+        <v>637</v>
+      </c>
+      <c r="M61" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5345,8 +6955,29 @@
       <c r="E62">
         <v>4392</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>574</v>
+      </c>
+      <c r="G62" t="s">
+        <v>574</v>
+      </c>
+      <c r="H62" t="s">
+        <v>573</v>
+      </c>
+      <c r="I62" t="s">
+        <v>573</v>
+      </c>
+      <c r="J62" t="s">
+        <v>574</v>
+      </c>
+      <c r="K62" t="s">
+        <v>573</v>
+      </c>
+      <c r="L62" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5362,8 +6993,29 @@
       <c r="E63">
         <v>4374</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>574</v>
+      </c>
+      <c r="G63" t="s">
+        <v>612</v>
+      </c>
+      <c r="H63" t="s">
+        <v>573</v>
+      </c>
+      <c r="I63" t="s">
+        <v>573</v>
+      </c>
+      <c r="J63" t="s">
+        <v>574</v>
+      </c>
+      <c r="K63" t="s">
+        <v>573</v>
+      </c>
+      <c r="L63" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5379,8 +7031,29 @@
       <c r="E64">
         <v>4364</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>574</v>
+      </c>
+      <c r="G64" t="s">
+        <v>612</v>
+      </c>
+      <c r="H64" t="s">
+        <v>573</v>
+      </c>
+      <c r="I64" t="s">
+        <v>573</v>
+      </c>
+      <c r="J64" t="s">
+        <v>574</v>
+      </c>
+      <c r="K64" t="s">
+        <v>573</v>
+      </c>
+      <c r="L64" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5396,8 +7069,29 @@
       <c r="E65">
         <v>4362</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>573</v>
+      </c>
+      <c r="G65" t="s">
+        <v>574</v>
+      </c>
+      <c r="H65" t="s">
+        <v>573</v>
+      </c>
+      <c r="I65" t="s">
+        <v>573</v>
+      </c>
+      <c r="J65" t="s">
+        <v>574</v>
+      </c>
+      <c r="K65" t="s">
+        <v>573</v>
+      </c>
+      <c r="L65" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5413,8 +7107,29 @@
       <c r="E66">
         <v>4323</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>574</v>
+      </c>
+      <c r="G66" t="s">
+        <v>574</v>
+      </c>
+      <c r="H66" t="s">
+        <v>573</v>
+      </c>
+      <c r="I66" t="s">
+        <v>573</v>
+      </c>
+      <c r="J66" t="s">
+        <v>574</v>
+      </c>
+      <c r="K66" t="s">
+        <v>573</v>
+      </c>
+      <c r="L66" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5430,8 +7145,29 @@
       <c r="E67">
         <v>4306</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>574</v>
+      </c>
+      <c r="G67" t="s">
+        <v>574</v>
+      </c>
+      <c r="H67" t="s">
+        <v>573</v>
+      </c>
+      <c r="I67" t="s">
+        <v>573</v>
+      </c>
+      <c r="J67" t="s">
+        <v>574</v>
+      </c>
+      <c r="K67" t="s">
+        <v>573</v>
+      </c>
+      <c r="L67" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5448,7 +7184,7 @@
         <v>4295</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5465,7 +7201,7 @@
         <v>4251</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5482,7 +7218,7 @@
         <v>4244</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5499,7 +7235,7 @@
         <v>4231</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5516,7 +7252,7 @@
         <v>4221</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5533,7 +7269,7 @@
         <v>4216</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5550,7 +7286,7 @@
         <v>4196</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5567,7 +7303,7 @@
         <v>4189</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5584,7 +7320,7 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5601,7 +7337,7 @@
         <v>4184</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5618,7 +7354,7 @@
         <v>4170</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5635,7 +7371,7 @@
         <v>4167</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
updates to excel file for abstracts
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0B33B1-CD9B-D347-85A2-51CA41A0E6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885C97DA-A521-4445-8D0C-6B84331DDB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="760" windowWidth="26140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44000" yWindow="820" windowWidth="24260" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="718">
   <si>
     <t>type</t>
   </si>
@@ -4077,6 +4077,9 @@
     <t>non-Latin char; includes hyperlinks</t>
   </si>
   <si>
+    <t>front matter</t>
+  </si>
+  <si>
     <t>front matter; includes personal contact information</t>
   </si>
   <si>
@@ -4219,6 +4222,99 @@
   </si>
   <si>
     <t>introduction</t>
+  </si>
+  <si>
+    <t>letters to the editor</t>
+  </si>
+  <si>
+    <t>book-chapter</t>
+  </si>
+  <si>
+    <t>proceedings abstract</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Editorial</t>
+  </si>
+  <si>
+    <t>Surrogatendpunkte</t>
+  </si>
+  <si>
+    <t>"pt"</t>
+  </si>
+  <si>
+    <t>article has both "pt" and "en" abstracts</t>
+  </si>
+  <si>
+    <t>"ar"</t>
+  </si>
+  <si>
+    <t>bibliography</t>
+  </si>
+  <si>
+    <t>editorial</t>
+  </si>
+  <si>
+    <t>the article is an abstract</t>
+  </si>
+  <si>
+    <t>proceedings preface</t>
+  </si>
+  <si>
+    <t>op-ed</t>
+  </si>
+  <si>
+    <t>abstract is in article</t>
+  </si>
+  <si>
+    <t>"de","en"</t>
+  </si>
+  <si>
+    <t>full review</t>
+  </si>
+  <si>
+    <t>the most egregious example of neglegence</t>
+  </si>
+  <si>
+    <t>Landing page has abstract, but article does not.</t>
+  </si>
+  <si>
+    <t>correction</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>biblio information; abstract in article and landing page</t>
+  </si>
+  <si>
+    <t>abstract in "ru" on landing page and in article</t>
+  </si>
+  <si>
+    <t>hiragana, katakana, CJK Ideograph, latin</t>
+  </si>
+  <si>
+    <t>"de"</t>
+  </si>
+  <si>
+    <t>"en" attribute but in "de"</t>
+  </si>
+  <si>
+    <t>no abstract in article</t>
+  </si>
+  <si>
+    <t>"tr"</t>
+  </si>
+  <si>
+    <t>article title used as abstract</t>
+  </si>
+  <si>
+    <t>section title used as abstract</t>
+  </si>
+  <si>
+    <t>"tr" attribute but editorial in "en"</t>
   </si>
 </sst>
 </file>
@@ -4296,7 +4392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4312,6 +4408,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4616,10 +4715,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C127" sqref="C127"/>
+      <selection pane="bottomLeft" activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7271,7 +7370,7 @@
         <v>573</v>
       </c>
       <c r="L66" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -7309,7 +7408,7 @@
         <v>573</v>
       </c>
       <c r="L67" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -7350,7 +7449,7 @@
         <v>615</v>
       </c>
       <c r="M68" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -7429,7 +7528,7 @@
         <v>595</v>
       </c>
       <c r="M70" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -7467,10 +7566,10 @@
         <v>573</v>
       </c>
       <c r="L71" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M71" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
@@ -7552,7 +7651,7 @@
         <v>616</v>
       </c>
       <c r="M73" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
@@ -7590,7 +7689,7 @@
         <v>573</v>
       </c>
       <c r="L74" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
@@ -7628,10 +7727,10 @@
         <v>573</v>
       </c>
       <c r="L75" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M75" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
@@ -7669,10 +7768,10 @@
         <v>573</v>
       </c>
       <c r="L76" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="M76" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
@@ -7713,7 +7812,7 @@
         <v>637</v>
       </c>
       <c r="M77" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -7754,7 +7853,7 @@
         <v>615</v>
       </c>
       <c r="M78" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
@@ -7982,7 +8081,7 @@
         <v>573</v>
       </c>
       <c r="L84" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -8058,10 +8157,10 @@
         <v>573</v>
       </c>
       <c r="L86" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M86" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -8099,10 +8198,10 @@
         <v>573</v>
       </c>
       <c r="L87" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M87" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -8181,7 +8280,7 @@
         <v>633</v>
       </c>
       <c r="M89" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -8219,10 +8318,10 @@
         <v>573</v>
       </c>
       <c r="L90" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M90" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -8298,10 +8397,10 @@
         <v>573</v>
       </c>
       <c r="L92" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M92" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -8342,7 +8441,7 @@
         <v>595</v>
       </c>
       <c r="M93" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -8494,10 +8593,10 @@
         <v>573</v>
       </c>
       <c r="L97" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="M97" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -8538,7 +8637,7 @@
         <v>615</v>
       </c>
       <c r="M98" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -8655,7 +8754,7 @@
         <v>615</v>
       </c>
       <c r="M101" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -8693,10 +8792,10 @@
         <v>573</v>
       </c>
       <c r="L102" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="M102" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -8734,10 +8833,10 @@
         <v>573</v>
       </c>
       <c r="L103" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="M103" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -8775,7 +8874,7 @@
         <v>573</v>
       </c>
       <c r="L104" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -8813,7 +8912,7 @@
         <v>573</v>
       </c>
       <c r="L105" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -8851,10 +8950,10 @@
         <v>573</v>
       </c>
       <c r="L106" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="M106" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -8892,7 +8991,7 @@
         <v>573</v>
       </c>
       <c r="L107" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -8930,7 +9029,7 @@
         <v>573</v>
       </c>
       <c r="L108" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -8953,7 +9052,7 @@
         <v>574</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H109" s="6" t="s">
         <v>574</v>
@@ -8968,10 +9067,10 @@
         <v>574</v>
       </c>
       <c r="L109" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="M109" s="6" t="s">
         <v>667</v>
-      </c>
-      <c r="M109" s="6" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
@@ -8994,7 +9093,7 @@
         <v>574</v>
       </c>
       <c r="G110" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H110" t="s">
         <v>574</v>
@@ -9009,10 +9108,10 @@
         <v>573</v>
       </c>
       <c r="L110" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="M110" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -9050,7 +9149,7 @@
         <v>573</v>
       </c>
       <c r="L111" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -9073,7 +9172,7 @@
         <v>574</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H112" t="s">
         <v>573</v>
@@ -9088,10 +9187,10 @@
         <v>574</v>
       </c>
       <c r="L112" t="s">
+        <v>672</v>
+      </c>
+      <c r="M112" t="s">
         <v>671</v>
-      </c>
-      <c r="M112" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
@@ -9129,10 +9228,10 @@
         <v>573</v>
       </c>
       <c r="L113" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="M113" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
@@ -9155,7 +9254,7 @@
         <v>574</v>
       </c>
       <c r="G114" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="H114" t="s">
         <v>573</v>
@@ -9170,7 +9269,7 @@
         <v>573</v>
       </c>
       <c r="L114" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
@@ -9193,7 +9292,7 @@
         <v>574</v>
       </c>
       <c r="G115" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H115" t="s">
         <v>591</v>
@@ -9208,7 +9307,7 @@
         <v>573</v>
       </c>
       <c r="L115" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
@@ -9246,10 +9345,10 @@
         <v>573</v>
       </c>
       <c r="L116" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="M116" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -9287,7 +9386,7 @@
         <v>573</v>
       </c>
       <c r="L117" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
@@ -9310,7 +9409,7 @@
         <v>574</v>
       </c>
       <c r="G118" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="H118" t="s">
         <v>574</v>
@@ -9325,10 +9424,10 @@
         <v>574</v>
       </c>
       <c r="L118" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="M118" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
@@ -9366,7 +9465,7 @@
         <v>573</v>
       </c>
       <c r="L119" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.2">
@@ -9389,7 +9488,7 @@
         <v>574</v>
       </c>
       <c r="G120" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="H120" t="s">
         <v>573</v>
@@ -9404,7 +9503,7 @@
         <v>573</v>
       </c>
       <c r="L120" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
@@ -9442,10 +9541,10 @@
         <v>573</v>
       </c>
       <c r="L121" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="M121" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
@@ -9483,7 +9582,7 @@
         <v>573</v>
       </c>
       <c r="L122" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
@@ -9521,7 +9620,7 @@
         <v>573</v>
       </c>
       <c r="L123" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
@@ -9559,7 +9658,7 @@
         <v>573</v>
       </c>
       <c r="L124" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
@@ -9597,10 +9696,10 @@
         <v>573</v>
       </c>
       <c r="L125" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="M125" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
@@ -9623,7 +9722,7 @@
         <v>574</v>
       </c>
       <c r="G126" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H126" t="s">
         <v>573</v>
@@ -9638,10 +9737,10 @@
         <v>573</v>
       </c>
       <c r="L126" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="M126" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
@@ -9660,6 +9759,27 @@
       <c r="E127">
         <v>18</v>
       </c>
+      <c r="F127" t="s">
+        <v>574</v>
+      </c>
+      <c r="G127" t="s">
+        <v>574</v>
+      </c>
+      <c r="H127" t="s">
+        <v>573</v>
+      </c>
+      <c r="I127" t="s">
+        <v>573</v>
+      </c>
+      <c r="J127" t="s">
+        <v>574</v>
+      </c>
+      <c r="K127" t="s">
+        <v>573</v>
+      </c>
+      <c r="L127" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
@@ -9677,8 +9797,29 @@
       <c r="E128">
         <v>18</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128" t="s">
+        <v>574</v>
+      </c>
+      <c r="G128" t="s">
+        <v>574</v>
+      </c>
+      <c r="H128" t="s">
+        <v>573</v>
+      </c>
+      <c r="I128" t="s">
+        <v>573</v>
+      </c>
+      <c r="J128" t="s">
+        <v>574</v>
+      </c>
+      <c r="K128" t="s">
+        <v>573</v>
+      </c>
+      <c r="L128" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -9694,8 +9835,32 @@
       <c r="E129">
         <v>18</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129" t="s">
+        <v>574</v>
+      </c>
+      <c r="G129" t="s">
+        <v>574</v>
+      </c>
+      <c r="H129" t="s">
+        <v>573</v>
+      </c>
+      <c r="I129" t="s">
+        <v>591</v>
+      </c>
+      <c r="J129" t="s">
+        <v>574</v>
+      </c>
+      <c r="K129" t="s">
+        <v>573</v>
+      </c>
+      <c r="L129" t="s">
+        <v>665</v>
+      </c>
+      <c r="M129" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -9711,8 +9876,32 @@
       <c r="E130">
         <v>18</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130" t="s">
+        <v>574</v>
+      </c>
+      <c r="G130" t="s">
+        <v>574</v>
+      </c>
+      <c r="H130" t="s">
+        <v>573</v>
+      </c>
+      <c r="I130" t="s">
+        <v>573</v>
+      </c>
+      <c r="J130" t="s">
+        <v>574</v>
+      </c>
+      <c r="K130" t="s">
+        <v>573</v>
+      </c>
+      <c r="L130" t="s">
+        <v>665</v>
+      </c>
+      <c r="M130" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -9728,8 +9917,29 @@
       <c r="E131">
         <v>18</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131" t="s">
+        <v>574</v>
+      </c>
+      <c r="G131" t="s">
+        <v>574</v>
+      </c>
+      <c r="H131" t="s">
+        <v>573</v>
+      </c>
+      <c r="I131" t="s">
+        <v>591</v>
+      </c>
+      <c r="J131" t="s">
+        <v>574</v>
+      </c>
+      <c r="K131" t="s">
+        <v>573</v>
+      </c>
+      <c r="L131" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -9745,8 +9955,32 @@
       <c r="E132">
         <v>18</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132" t="s">
+        <v>574</v>
+      </c>
+      <c r="G132" t="s">
+        <v>574</v>
+      </c>
+      <c r="H132" t="s">
+        <v>573</v>
+      </c>
+      <c r="I132" t="s">
+        <v>573</v>
+      </c>
+      <c r="J132" t="s">
+        <v>574</v>
+      </c>
+      <c r="K132" t="s">
+        <v>573</v>
+      </c>
+      <c r="L132" t="s">
+        <v>665</v>
+      </c>
+      <c r="M132" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -9762,8 +9996,32 @@
       <c r="E133">
         <v>19</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133" t="s">
+        <v>574</v>
+      </c>
+      <c r="G133" t="s">
+        <v>574</v>
+      </c>
+      <c r="H133" t="s">
+        <v>573</v>
+      </c>
+      <c r="I133" t="s">
+        <v>574</v>
+      </c>
+      <c r="J133" t="s">
+        <v>574</v>
+      </c>
+      <c r="K133" t="s">
+        <v>573</v>
+      </c>
+      <c r="L133" t="s">
+        <v>681</v>
+      </c>
+      <c r="M133" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -9779,8 +10037,29 @@
       <c r="E134">
         <v>20</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134" t="s">
+        <v>574</v>
+      </c>
+      <c r="G134" t="s">
+        <v>574</v>
+      </c>
+      <c r="H134" t="s">
+        <v>573</v>
+      </c>
+      <c r="I134" t="s">
+        <v>573</v>
+      </c>
+      <c r="J134" t="s">
+        <v>574</v>
+      </c>
+      <c r="K134" t="s">
+        <v>573</v>
+      </c>
+      <c r="L134" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -9796,8 +10075,32 @@
       <c r="E135">
         <v>20</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135" t="s">
+        <v>574</v>
+      </c>
+      <c r="G135" t="s">
+        <v>574</v>
+      </c>
+      <c r="H135" t="s">
+        <v>573</v>
+      </c>
+      <c r="I135" t="s">
+        <v>573</v>
+      </c>
+      <c r="J135" t="s">
+        <v>574</v>
+      </c>
+      <c r="K135" t="s">
+        <v>573</v>
+      </c>
+      <c r="L135" t="s">
+        <v>665</v>
+      </c>
+      <c r="M135" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -9813,8 +10116,29 @@
       <c r="E136">
         <v>20</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136" t="s">
+        <v>574</v>
+      </c>
+      <c r="G136" t="s">
+        <v>574</v>
+      </c>
+      <c r="H136" t="s">
+        <v>573</v>
+      </c>
+      <c r="I136" t="s">
+        <v>573</v>
+      </c>
+      <c r="J136" t="s">
+        <v>574</v>
+      </c>
+      <c r="K136" t="s">
+        <v>573</v>
+      </c>
+      <c r="L136" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -9830,8 +10154,32 @@
       <c r="E137">
         <v>20</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137" t="s">
+        <v>574</v>
+      </c>
+      <c r="G137" t="s">
+        <v>574</v>
+      </c>
+      <c r="H137" t="s">
+        <v>573</v>
+      </c>
+      <c r="I137" t="s">
+        <v>573</v>
+      </c>
+      <c r="J137" t="s">
+        <v>574</v>
+      </c>
+      <c r="K137" t="s">
+        <v>573</v>
+      </c>
+      <c r="L137" t="s">
+        <v>665</v>
+      </c>
+      <c r="M137" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -9847,8 +10195,32 @@
       <c r="E138">
         <v>20</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138" t="s">
+        <v>574</v>
+      </c>
+      <c r="G138" t="s">
+        <v>574</v>
+      </c>
+      <c r="H138" t="s">
+        <v>573</v>
+      </c>
+      <c r="I138" t="s">
+        <v>573</v>
+      </c>
+      <c r="J138" t="s">
+        <v>574</v>
+      </c>
+      <c r="K138" t="s">
+        <v>573</v>
+      </c>
+      <c r="L138" t="s">
+        <v>665</v>
+      </c>
+      <c r="M138" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -9864,25 +10236,70 @@
       <c r="E139">
         <v>20</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="1">
+      <c r="F139" t="s">
+        <v>574</v>
+      </c>
+      <c r="G139" t="s">
+        <v>574</v>
+      </c>
+      <c r="H139" t="s">
+        <v>591</v>
+      </c>
+      <c r="I139" t="s">
+        <v>573</v>
+      </c>
+      <c r="J139" t="s">
+        <v>574</v>
+      </c>
+      <c r="K139" t="s">
+        <v>573</v>
+      </c>
+      <c r="L139" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A140" s="7">
         <v>138</v>
       </c>
-      <c r="B140" t="s">
-        <v>4</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="B140" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="6">
         <v>21</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>693</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="I140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="J140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="K140" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="L140" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="M140" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -9898,8 +10315,29 @@
       <c r="E141">
         <v>23</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141" t="s">
+        <v>574</v>
+      </c>
+      <c r="G141" t="s">
+        <v>574</v>
+      </c>
+      <c r="H141" t="s">
+        <v>573</v>
+      </c>
+      <c r="I141" t="s">
+        <v>573</v>
+      </c>
+      <c r="J141" t="s">
+        <v>574</v>
+      </c>
+      <c r="K141" t="s">
+        <v>573</v>
+      </c>
+      <c r="L141" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -9915,8 +10353,29 @@
       <c r="E142">
         <v>23</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142" t="s">
+        <v>574</v>
+      </c>
+      <c r="G142" t="s">
+        <v>574</v>
+      </c>
+      <c r="H142" t="s">
+        <v>573</v>
+      </c>
+      <c r="I142" t="s">
+        <v>573</v>
+      </c>
+      <c r="J142" t="s">
+        <v>574</v>
+      </c>
+      <c r="K142" t="s">
+        <v>573</v>
+      </c>
+      <c r="L142" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -9932,8 +10391,29 @@
       <c r="E143">
         <v>23</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143" t="s">
+        <v>574</v>
+      </c>
+      <c r="G143" t="s">
+        <v>574</v>
+      </c>
+      <c r="H143" t="s">
+        <v>573</v>
+      </c>
+      <c r="I143" t="s">
+        <v>573</v>
+      </c>
+      <c r="J143" t="s">
+        <v>574</v>
+      </c>
+      <c r="K143" t="s">
+        <v>573</v>
+      </c>
+      <c r="L143" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -9949,8 +10429,29 @@
       <c r="E144">
         <v>24</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144" t="s">
+        <v>574</v>
+      </c>
+      <c r="G144" t="s">
+        <v>695</v>
+      </c>
+      <c r="H144" t="s">
+        <v>573</v>
+      </c>
+      <c r="I144" t="s">
+        <v>573</v>
+      </c>
+      <c r="J144" t="s">
+        <v>574</v>
+      </c>
+      <c r="K144" t="s">
+        <v>573</v>
+      </c>
+      <c r="L144" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -9966,8 +10467,32 @@
       <c r="E145">
         <v>25</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145" t="s">
+        <v>574</v>
+      </c>
+      <c r="G145" t="s">
+        <v>574</v>
+      </c>
+      <c r="H145" t="s">
+        <v>573</v>
+      </c>
+      <c r="I145" t="s">
+        <v>591</v>
+      </c>
+      <c r="J145" t="s">
+        <v>574</v>
+      </c>
+      <c r="K145" t="s">
+        <v>573</v>
+      </c>
+      <c r="L145" t="s">
+        <v>659</v>
+      </c>
+      <c r="M145" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -9983,8 +10508,29 @@
       <c r="E146">
         <v>26</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146" t="s">
+        <v>574</v>
+      </c>
+      <c r="G146" t="s">
+        <v>574</v>
+      </c>
+      <c r="H146" t="s">
+        <v>573</v>
+      </c>
+      <c r="I146" t="s">
+        <v>573</v>
+      </c>
+      <c r="J146" t="s">
+        <v>574</v>
+      </c>
+      <c r="K146" t="s">
+        <v>573</v>
+      </c>
+      <c r="L146" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -10000,8 +10546,32 @@
       <c r="E147">
         <v>26</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147" t="s">
+        <v>574</v>
+      </c>
+      <c r="G147" t="s">
+        <v>574</v>
+      </c>
+      <c r="H147" t="s">
+        <v>573</v>
+      </c>
+      <c r="I147" t="s">
+        <v>573</v>
+      </c>
+      <c r="J147" t="s">
+        <v>574</v>
+      </c>
+      <c r="K147" t="s">
+        <v>573</v>
+      </c>
+      <c r="L147" t="s">
+        <v>665</v>
+      </c>
+      <c r="M147" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -10017,8 +10587,29 @@
       <c r="E148">
         <v>26</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148" t="s">
+        <v>574</v>
+      </c>
+      <c r="G148" t="s">
+        <v>574</v>
+      </c>
+      <c r="H148" t="s">
+        <v>573</v>
+      </c>
+      <c r="I148" t="s">
+        <v>573</v>
+      </c>
+      <c r="J148" t="s">
+        <v>574</v>
+      </c>
+      <c r="K148" t="s">
+        <v>573</v>
+      </c>
+      <c r="L148" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -10034,8 +10625,29 @@
       <c r="E149">
         <v>26</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F149" t="s">
+        <v>574</v>
+      </c>
+      <c r="G149" t="s">
+        <v>574</v>
+      </c>
+      <c r="H149" t="s">
+        <v>573</v>
+      </c>
+      <c r="I149" t="s">
+        <v>573</v>
+      </c>
+      <c r="J149" t="s">
+        <v>574</v>
+      </c>
+      <c r="K149" t="s">
+        <v>573</v>
+      </c>
+      <c r="L149" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -10051,8 +10663,29 @@
       <c r="E150">
         <v>26</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F150" t="s">
+        <v>574</v>
+      </c>
+      <c r="G150" t="s">
+        <v>574</v>
+      </c>
+      <c r="H150" t="s">
+        <v>573</v>
+      </c>
+      <c r="I150" t="s">
+        <v>573</v>
+      </c>
+      <c r="J150" t="s">
+        <v>574</v>
+      </c>
+      <c r="K150" t="s">
+        <v>573</v>
+      </c>
+      <c r="L150" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -10068,8 +10701,32 @@
       <c r="E151">
         <v>29</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F151" t="s">
+        <v>574</v>
+      </c>
+      <c r="G151" t="s">
+        <v>574</v>
+      </c>
+      <c r="H151" t="s">
+        <v>573</v>
+      </c>
+      <c r="I151" t="s">
+        <v>573</v>
+      </c>
+      <c r="J151" t="s">
+        <v>574</v>
+      </c>
+      <c r="K151" t="s">
+        <v>573</v>
+      </c>
+      <c r="L151" t="s">
+        <v>659</v>
+      </c>
+      <c r="M151" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -10085,8 +10742,32 @@
       <c r="E152">
         <v>30</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F152" t="s">
+        <v>574</v>
+      </c>
+      <c r="G152" t="s">
+        <v>574</v>
+      </c>
+      <c r="H152" t="s">
+        <v>573</v>
+      </c>
+      <c r="I152" t="s">
+        <v>574</v>
+      </c>
+      <c r="J152" t="s">
+        <v>574</v>
+      </c>
+      <c r="K152" t="s">
+        <v>573</v>
+      </c>
+      <c r="L152" t="s">
+        <v>681</v>
+      </c>
+      <c r="M152" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -10102,8 +10783,29 @@
       <c r="E153">
         <v>32</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F153" t="s">
+        <v>574</v>
+      </c>
+      <c r="G153" t="s">
+        <v>574</v>
+      </c>
+      <c r="H153" t="s">
+        <v>573</v>
+      </c>
+      <c r="I153" t="s">
+        <v>573</v>
+      </c>
+      <c r="J153" t="s">
+        <v>574</v>
+      </c>
+      <c r="K153" t="s">
+        <v>573</v>
+      </c>
+      <c r="L153" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -10119,8 +10821,32 @@
       <c r="E154">
         <v>38</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F154" t="s">
+        <v>574</v>
+      </c>
+      <c r="G154" t="s">
+        <v>574</v>
+      </c>
+      <c r="H154" t="s">
+        <v>573</v>
+      </c>
+      <c r="I154" t="s">
+        <v>573</v>
+      </c>
+      <c r="J154" t="s">
+        <v>574</v>
+      </c>
+      <c r="K154" t="s">
+        <v>573</v>
+      </c>
+      <c r="L154" t="s">
+        <v>665</v>
+      </c>
+      <c r="M154" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -10136,8 +10862,29 @@
       <c r="E155">
         <v>39</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F155" t="s">
+        <v>574</v>
+      </c>
+      <c r="G155" t="s">
+        <v>574</v>
+      </c>
+      <c r="H155" t="s">
+        <v>573</v>
+      </c>
+      <c r="I155" t="s">
+        <v>573</v>
+      </c>
+      <c r="J155" t="s">
+        <v>574</v>
+      </c>
+      <c r="K155" t="s">
+        <v>573</v>
+      </c>
+      <c r="L155" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -10153,8 +10900,32 @@
       <c r="E156">
         <v>44</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F156" t="s">
+        <v>574</v>
+      </c>
+      <c r="G156" t="s">
+        <v>574</v>
+      </c>
+      <c r="H156" t="s">
+        <v>573</v>
+      </c>
+      <c r="I156" t="s">
+        <v>573</v>
+      </c>
+      <c r="J156" t="s">
+        <v>574</v>
+      </c>
+      <c r="K156" t="s">
+        <v>573</v>
+      </c>
+      <c r="L156" t="s">
+        <v>665</v>
+      </c>
+      <c r="M156" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -10170,8 +10941,32 @@
       <c r="E157">
         <v>44</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F157" t="s">
+        <v>574</v>
+      </c>
+      <c r="G157" t="s">
+        <v>574</v>
+      </c>
+      <c r="H157" t="s">
+        <v>573</v>
+      </c>
+      <c r="I157" t="s">
+        <v>574</v>
+      </c>
+      <c r="J157" t="s">
+        <v>574</v>
+      </c>
+      <c r="K157" t="s">
+        <v>573</v>
+      </c>
+      <c r="L157" t="s">
+        <v>681</v>
+      </c>
+      <c r="M157" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -10187,8 +10982,32 @@
       <c r="E158">
         <v>45</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F158" t="s">
+        <v>574</v>
+      </c>
+      <c r="G158" t="s">
+        <v>702</v>
+      </c>
+      <c r="H158" t="s">
+        <v>573</v>
+      </c>
+      <c r="I158" t="s">
+        <v>573</v>
+      </c>
+      <c r="J158" t="s">
+        <v>574</v>
+      </c>
+      <c r="K158" t="s">
+        <v>573</v>
+      </c>
+      <c r="L158" t="s">
+        <v>665</v>
+      </c>
+      <c r="M158" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -10204,8 +11023,32 @@
       <c r="E159">
         <v>48</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F159" t="s">
+        <v>574</v>
+      </c>
+      <c r="G159" t="s">
+        <v>574</v>
+      </c>
+      <c r="H159" t="s">
+        <v>573</v>
+      </c>
+      <c r="I159" t="s">
+        <v>573</v>
+      </c>
+      <c r="J159" t="s">
+        <v>574</v>
+      </c>
+      <c r="K159" t="s">
+        <v>573</v>
+      </c>
+      <c r="L159" t="s">
+        <v>665</v>
+      </c>
+      <c r="M159" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -10221,42 +11064,114 @@
       <c r="E160">
         <v>48</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="1">
+      <c r="F160" t="s">
+        <v>574</v>
+      </c>
+      <c r="G160" t="s">
+        <v>574</v>
+      </c>
+      <c r="H160" t="s">
+        <v>573</v>
+      </c>
+      <c r="I160" t="s">
+        <v>573</v>
+      </c>
+      <c r="J160" t="s">
+        <v>574</v>
+      </c>
+      <c r="K160" t="s">
+        <v>573</v>
+      </c>
+      <c r="L160" t="s">
+        <v>665</v>
+      </c>
+      <c r="M160" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A161" s="7">
         <v>159</v>
       </c>
-      <c r="B161" t="s">
-        <v>4</v>
-      </c>
-      <c r="C161" t="s">
+      <c r="B161" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C161" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E161">
+      <c r="E161" s="6">
         <v>49</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" s="1">
+      <c r="F161" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="G161" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="H161" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="I161" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="J161" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="K161" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="L161" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="M161" s="6" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A162" s="7">
         <v>160</v>
       </c>
-      <c r="B162" t="s">
-        <v>4</v>
-      </c>
-      <c r="C162" t="s">
+      <c r="B162" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="E162">
+      <c r="E162" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F162" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="G162" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="H162" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="I162" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="J162" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="K162" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="L162" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="M162" s="6" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -10272,8 +11187,32 @@
       <c r="E163">
         <v>50</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F163" t="s">
+        <v>574</v>
+      </c>
+      <c r="G163" t="s">
+        <v>574</v>
+      </c>
+      <c r="H163" t="s">
+        <v>574</v>
+      </c>
+      <c r="I163" t="s">
+        <v>574</v>
+      </c>
+      <c r="J163" t="s">
+        <v>574</v>
+      </c>
+      <c r="K163" t="s">
+        <v>573</v>
+      </c>
+      <c r="L163" t="s">
+        <v>665</v>
+      </c>
+      <c r="M163" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -10289,8 +11228,32 @@
       <c r="E164">
         <v>51</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F164" t="s">
+        <v>574</v>
+      </c>
+      <c r="G164" t="s">
+        <v>574</v>
+      </c>
+      <c r="H164" t="s">
+        <v>573</v>
+      </c>
+      <c r="I164" t="s">
+        <v>573</v>
+      </c>
+      <c r="J164" t="s">
+        <v>574</v>
+      </c>
+      <c r="K164" t="s">
+        <v>573</v>
+      </c>
+      <c r="L164" t="s">
+        <v>665</v>
+      </c>
+      <c r="M164" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -10306,8 +11269,29 @@
       <c r="E165">
         <v>52</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F165" t="s">
+        <v>574</v>
+      </c>
+      <c r="G165" t="s">
+        <v>574</v>
+      </c>
+      <c r="H165" t="s">
+        <v>573</v>
+      </c>
+      <c r="I165" t="s">
+        <v>573</v>
+      </c>
+      <c r="J165" t="s">
+        <v>574</v>
+      </c>
+      <c r="K165" t="s">
+        <v>573</v>
+      </c>
+      <c r="L165" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -10323,8 +11307,29 @@
       <c r="E166">
         <v>54</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F166" t="s">
+        <v>574</v>
+      </c>
+      <c r="G166" t="s">
+        <v>574</v>
+      </c>
+      <c r="H166" t="s">
+        <v>591</v>
+      </c>
+      <c r="I166" t="s">
+        <v>591</v>
+      </c>
+      <c r="J166" t="s">
+        <v>574</v>
+      </c>
+      <c r="K166" t="s">
+        <v>573</v>
+      </c>
+      <c r="L166" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -10340,8 +11345,32 @@
       <c r="E167">
         <v>55</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F167" t="s">
+        <v>574</v>
+      </c>
+      <c r="G167" t="s">
+        <v>574</v>
+      </c>
+      <c r="H167" t="s">
+        <v>574</v>
+      </c>
+      <c r="I167" t="s">
+        <v>574</v>
+      </c>
+      <c r="J167" t="s">
+        <v>574</v>
+      </c>
+      <c r="K167" t="s">
+        <v>573</v>
+      </c>
+      <c r="L167" t="s">
+        <v>708</v>
+      </c>
+      <c r="M167" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -10357,8 +11386,32 @@
       <c r="E168">
         <v>56</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F168" t="s">
+        <v>574</v>
+      </c>
+      <c r="G168" t="s">
+        <v>574</v>
+      </c>
+      <c r="H168" t="s">
+        <v>573</v>
+      </c>
+      <c r="I168" t="s">
+        <v>591</v>
+      </c>
+      <c r="J168" t="s">
+        <v>574</v>
+      </c>
+      <c r="K168" t="s">
+        <v>573</v>
+      </c>
+      <c r="L168" t="s">
+        <v>595</v>
+      </c>
+      <c r="M168" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -10374,8 +11427,29 @@
       <c r="E169">
         <v>57</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169" t="s">
+        <v>574</v>
+      </c>
+      <c r="G169" t="s">
+        <v>711</v>
+      </c>
+      <c r="H169" t="s">
+        <v>573</v>
+      </c>
+      <c r="I169" t="s">
+        <v>591</v>
+      </c>
+      <c r="J169" t="s">
+        <v>573</v>
+      </c>
+      <c r="K169" t="s">
+        <v>573</v>
+      </c>
+      <c r="L169" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -10391,8 +11465,32 @@
       <c r="E170">
         <v>58</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F170" t="s">
+        <v>574</v>
+      </c>
+      <c r="G170" t="s">
+        <v>612</v>
+      </c>
+      <c r="H170" t="s">
+        <v>573</v>
+      </c>
+      <c r="I170" t="s">
+        <v>573</v>
+      </c>
+      <c r="J170" t="s">
+        <v>574</v>
+      </c>
+      <c r="K170" t="s">
+        <v>573</v>
+      </c>
+      <c r="L170" t="s">
+        <v>716</v>
+      </c>
+      <c r="M170" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -10408,8 +11506,32 @@
       <c r="E171">
         <v>58</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F171" t="s">
+        <v>574</v>
+      </c>
+      <c r="G171" t="s">
+        <v>714</v>
+      </c>
+      <c r="H171" t="s">
+        <v>573</v>
+      </c>
+      <c r="I171" t="s">
+        <v>573</v>
+      </c>
+      <c r="J171" t="s">
+        <v>574</v>
+      </c>
+      <c r="K171" t="s">
+        <v>573</v>
+      </c>
+      <c r="L171" t="s">
+        <v>715</v>
+      </c>
+      <c r="M171" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -10425,8 +11547,29 @@
       <c r="E172">
         <v>58</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F172" t="s">
+        <v>574</v>
+      </c>
+      <c r="G172" t="s">
+        <v>574</v>
+      </c>
+      <c r="H172" t="s">
+        <v>573</v>
+      </c>
+      <c r="I172" t="s">
+        <v>573</v>
+      </c>
+      <c r="J172" t="s">
+        <v>574</v>
+      </c>
+      <c r="K172" t="s">
+        <v>573</v>
+      </c>
+      <c r="L172" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -10442,8 +11585,29 @@
       <c r="E173">
         <v>59</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173" t="s">
+        <v>574</v>
+      </c>
+      <c r="G173" t="s">
+        <v>612</v>
+      </c>
+      <c r="H173" t="s">
+        <v>573</v>
+      </c>
+      <c r="I173" t="s">
+        <v>573</v>
+      </c>
+      <c r="J173" t="s">
+        <v>574</v>
+      </c>
+      <c r="K173" t="s">
+        <v>573</v>
+      </c>
+      <c r="L173" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -10459,8 +11623,29 @@
       <c r="E174">
         <v>59</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174" t="s">
+        <v>574</v>
+      </c>
+      <c r="G174" t="s">
+        <v>612</v>
+      </c>
+      <c r="H174" t="s">
+        <v>573</v>
+      </c>
+      <c r="I174" t="s">
+        <v>573</v>
+      </c>
+      <c r="J174" t="s">
+        <v>574</v>
+      </c>
+      <c r="K174" t="s">
+        <v>573</v>
+      </c>
+      <c r="L174" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -10476,8 +11661,29 @@
       <c r="E175">
         <v>59</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175" t="s">
+        <v>574</v>
+      </c>
+      <c r="G175" t="s">
+        <v>612</v>
+      </c>
+      <c r="H175" t="s">
+        <v>573</v>
+      </c>
+      <c r="I175" t="s">
+        <v>573</v>
+      </c>
+      <c r="J175" t="s">
+        <v>574</v>
+      </c>
+      <c r="K175" t="s">
+        <v>573</v>
+      </c>
+      <c r="L175" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -10493,8 +11699,29 @@
       <c r="E176">
         <v>59</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176" t="s">
+        <v>574</v>
+      </c>
+      <c r="G176" t="s">
+        <v>612</v>
+      </c>
+      <c r="H176" t="s">
+        <v>573</v>
+      </c>
+      <c r="I176" t="s">
+        <v>573</v>
+      </c>
+      <c r="J176" t="s">
+        <v>574</v>
+      </c>
+      <c r="K176" t="s">
+        <v>573</v>
+      </c>
+      <c r="L176" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -10510,8 +11737,29 @@
       <c r="E177">
         <v>59</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F177" t="s">
+        <v>574</v>
+      </c>
+      <c r="G177" t="s">
+        <v>612</v>
+      </c>
+      <c r="H177" t="s">
+        <v>573</v>
+      </c>
+      <c r="I177" t="s">
+        <v>573</v>
+      </c>
+      <c r="J177" t="s">
+        <v>574</v>
+      </c>
+      <c r="K177" t="s">
+        <v>573</v>
+      </c>
+      <c r="L177" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -10527,8 +11775,29 @@
       <c r="E178">
         <v>66</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F178" t="s">
+        <v>574</v>
+      </c>
+      <c r="G178" t="s">
+        <v>574</v>
+      </c>
+      <c r="H178" t="s">
+        <v>573</v>
+      </c>
+      <c r="I178" t="s">
+        <v>573</v>
+      </c>
+      <c r="J178" t="s">
+        <v>574</v>
+      </c>
+      <c r="K178" t="s">
+        <v>573</v>
+      </c>
+      <c r="L178" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -10544,8 +11813,32 @@
       <c r="E179">
         <v>68</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179" t="s">
+        <v>574</v>
+      </c>
+      <c r="G179" t="s">
+        <v>574</v>
+      </c>
+      <c r="H179" t="s">
+        <v>573</v>
+      </c>
+      <c r="I179" t="s">
+        <v>573</v>
+      </c>
+      <c r="J179" t="s">
+        <v>574</v>
+      </c>
+      <c r="K179" t="s">
+        <v>573</v>
+      </c>
+      <c r="L179" t="s">
+        <v>713</v>
+      </c>
+      <c r="M179" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -10562,7 +11855,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -10579,7 +11872,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -10596,7 +11889,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -10613,7 +11906,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -10630,7 +11923,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -10647,7 +11940,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -10664,7 +11957,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -10681,7 +11974,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -10698,7 +11991,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -10715,7 +12008,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -10732,7 +12025,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -10749,7 +12042,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
revised excel, improved corr
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B883329-294A-6746-A1C0-9B206C6F07E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B31678B-D4A6-EB41-A64B-0076A7F8201D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3880" yWindow="760" windowWidth="26140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="735">
   <si>
     <t>type</t>
   </si>
@@ -4071,9 +4071,6 @@
     <t xml:space="preserve">bad url </t>
   </si>
   <si>
-    <t>empty</t>
-  </si>
-  <si>
     <t>landing page in "en" and "ko"</t>
   </si>
   <si>
@@ -4369,9 +4366,6 @@
   </si>
   <si>
     <t>includes U+2009 Thin Space General Punc char</t>
-  </si>
-  <si>
-    <t xml:space="preserve">empty; </t>
   </si>
   <si>
     <t>HTML</t>
@@ -4475,28 +4469,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4796,10 +4769,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="L150" sqref="L150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4849,7 +4822,7 @@
         <v>598</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>570</v>
@@ -4875,7 +4848,7 @@
         <v>10871</v>
       </c>
       <c r="F2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G2" t="s">
         <v>574</v>
@@ -4896,7 +4869,7 @@
         <v>574</v>
       </c>
       <c r="M2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -4937,7 +4910,7 @@
         <v>574</v>
       </c>
       <c r="M3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -5063,10 +5036,10 @@
         <v>574</v>
       </c>
       <c r="M6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -5171,7 +5144,7 @@
         <v>6937</v>
       </c>
       <c r="F9" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G9" t="s">
         <v>574</v>
@@ -5192,7 +5165,7 @@
         <v>574</v>
       </c>
       <c r="M9" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="N9" t="s">
         <v>578</v>
@@ -5215,7 +5188,7 @@
         <v>6602</v>
       </c>
       <c r="F10" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G10" t="s">
         <v>573</v>
@@ -5236,7 +5209,7 @@
         <v>574</v>
       </c>
       <c r="M10" t="s">
-        <v>615</v>
+        <v>729</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -5256,7 +5229,7 @@
         <v>6576</v>
       </c>
       <c r="F11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G11" t="s">
         <v>574</v>
@@ -5277,7 +5250,7 @@
         <v>573</v>
       </c>
       <c r="M11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N11" t="s">
         <v>579</v>
@@ -5321,7 +5294,7 @@
         <v>573</v>
       </c>
       <c r="M12" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N12" t="s">
         <v>582</v>
@@ -5409,7 +5382,7 @@
         <v>573</v>
       </c>
       <c r="M14" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N14" t="s">
         <v>581</v>
@@ -5473,7 +5446,7 @@
         <v>5878</v>
       </c>
       <c r="F16" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G16" t="s">
         <v>574</v>
@@ -5491,10 +5464,10 @@
         <v>573</v>
       </c>
       <c r="L16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="M16" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="N16" t="s">
         <v>584</v>
@@ -5561,7 +5534,7 @@
         <v>5526</v>
       </c>
       <c r="F18" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G18" t="s">
         <v>574</v>
@@ -5626,7 +5599,7 @@
         <v>574</v>
       </c>
       <c r="M19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N19" t="s">
         <v>587</v>
@@ -5649,7 +5622,7 @@
         <v>5490</v>
       </c>
       <c r="F20" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G20" t="s">
         <v>574</v>
@@ -5670,7 +5643,7 @@
         <v>574</v>
       </c>
       <c r="M20" t="s">
-        <v>615</v>
+        <v>729</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -5711,7 +5684,7 @@
         <v>573</v>
       </c>
       <c r="M21" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N21" t="s">
         <v>588</v>
@@ -5755,7 +5728,7 @@
         <v>573</v>
       </c>
       <c r="M22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="N22" t="s">
         <v>580</v>
@@ -5778,7 +5751,7 @@
         <v>5272</v>
       </c>
       <c r="F23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G23" t="s">
         <v>574</v>
@@ -5799,7 +5772,7 @@
         <v>574</v>
       </c>
       <c r="M23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="N23" t="s">
         <v>589</v>
@@ -5822,7 +5795,7 @@
         <v>5209</v>
       </c>
       <c r="F24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G24" t="s">
         <v>574</v>
@@ -5910,7 +5883,7 @@
         <v>5162</v>
       </c>
       <c r="F26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G26" t="s">
         <v>574</v>
@@ -5928,10 +5901,10 @@
         <v>573</v>
       </c>
       <c r="L26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="M26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="N26" t="s">
         <v>580</v>
@@ -6233,7 +6206,7 @@
         <v>573</v>
       </c>
       <c r="M33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N33" t="s">
         <v>600</v>
@@ -6318,7 +6291,7 @@
         <v>573</v>
       </c>
       <c r="M35" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N35" t="s">
         <v>604</v>
@@ -6362,7 +6335,7 @@
         <v>573</v>
       </c>
       <c r="M36" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N36" t="s">
         <v>604</v>
@@ -6406,7 +6379,7 @@
         <v>573</v>
       </c>
       <c r="M37" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N37" t="s">
         <v>604</v>
@@ -6535,7 +6508,7 @@
         <v>573</v>
       </c>
       <c r="M40" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N40" t="s">
         <v>606</v>
@@ -6579,7 +6552,7 @@
         <v>573</v>
       </c>
       <c r="M41" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N41" t="s">
         <v>607</v>
@@ -6623,7 +6596,7 @@
         <v>573</v>
       </c>
       <c r="M42" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N42" t="s">
         <v>608</v>
@@ -6749,7 +6722,7 @@
         <v>573</v>
       </c>
       <c r="M45" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N45" t="s">
         <v>604</v>
@@ -6793,7 +6766,7 @@
         <v>574</v>
       </c>
       <c r="M46" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -7095,7 +7068,7 @@
         <v>573</v>
       </c>
       <c r="M53" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N53" t="s">
         <v>613</v>
@@ -7139,7 +7112,7 @@
         <v>573</v>
       </c>
       <c r="M54" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N54" t="s">
         <v>613</v>
@@ -7183,7 +7156,7 @@
         <v>573</v>
       </c>
       <c r="M55" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="N55" t="s">
         <v>612</v>
@@ -7227,7 +7200,7 @@
         <v>573</v>
       </c>
       <c r="M56" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="N56" t="s">
         <v>614</v>
@@ -7271,7 +7244,7 @@
         <v>573</v>
       </c>
       <c r="M57" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N57" t="s">
         <v>604</v>
@@ -7587,7 +7560,7 @@
         <v>4362</v>
       </c>
       <c r="F65" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G65" t="s">
         <v>574</v>
@@ -7608,7 +7581,7 @@
         <v>574</v>
       </c>
       <c r="M65" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -7731,7 +7704,7 @@
         <v>574</v>
       </c>
       <c r="M68" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N68" t="s">
         <v>621</v>
@@ -7775,7 +7748,7 @@
         <v>574</v>
       </c>
       <c r="M69" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -7860,7 +7833,7 @@
         <v>574</v>
       </c>
       <c r="M71" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N71" t="s">
         <v>623</v>
@@ -7904,7 +7877,7 @@
         <v>573</v>
       </c>
       <c r="M72" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N72" t="s">
         <v>604</v>
@@ -7948,7 +7921,7 @@
         <v>573</v>
       </c>
       <c r="M73" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N73" t="s">
         <v>624</v>
@@ -7992,7 +7965,7 @@
         <v>574</v>
       </c>
       <c r="M74" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -8033,7 +8006,7 @@
         <v>574</v>
       </c>
       <c r="M75" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N75" t="s">
         <v>623</v>
@@ -8056,7 +8029,7 @@
         <v>4185</v>
       </c>
       <c r="F76" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G76" t="s">
         <v>574</v>
@@ -8165,7 +8138,7 @@
         <v>574</v>
       </c>
       <c r="M78" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N78" t="s">
         <v>628</v>
@@ -8209,7 +8182,7 @@
         <v>574</v>
       </c>
       <c r="M79" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -8229,7 +8202,7 @@
         <v>4162</v>
       </c>
       <c r="F80" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G80" t="s">
         <v>601</v>
@@ -8250,7 +8223,7 @@
         <v>574</v>
       </c>
       <c r="M80" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -8455,7 +8428,7 @@
         <v>574</v>
       </c>
       <c r="M85" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -8475,7 +8448,7 @@
         <v>4100</v>
       </c>
       <c r="F86" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G86" t="s">
         <v>574</v>
@@ -8540,7 +8513,7 @@
         <v>574</v>
       </c>
       <c r="M87" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N87" t="s">
         <v>630</v>
@@ -8669,7 +8642,7 @@
         <v>574</v>
       </c>
       <c r="M90" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N90" t="s">
         <v>632</v>
@@ -8733,7 +8706,7 @@
         <v>4045</v>
       </c>
       <c r="F92" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G92" t="s">
         <v>601</v>
@@ -9009,7 +8982,7 @@
         <v>574</v>
       </c>
       <c r="M98" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N98" t="s">
         <v>633</v>
@@ -9135,7 +9108,7 @@
         <v>574</v>
       </c>
       <c r="M101" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N101" t="s">
         <v>634</v>
@@ -9179,10 +9152,10 @@
         <v>574</v>
       </c>
       <c r="M102" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N102" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -9223,10 +9196,10 @@
         <v>574</v>
       </c>
       <c r="M103" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N103" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -9349,10 +9322,10 @@
         <v>574</v>
       </c>
       <c r="M106" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N106" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -9393,10 +9366,10 @@
         <v>574</v>
       </c>
       <c r="M107" t="s">
-        <v>635</v>
+        <v>681</v>
       </c>
       <c r="N107" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -9437,7 +9410,7 @@
         <v>574</v>
       </c>
       <c r="M108" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -9460,28 +9433,28 @@
         <v>574</v>
       </c>
       <c r="G109" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="I109" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="J109" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="K109" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="L109" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="M109" t="s">
+        <v>643</v>
+      </c>
+      <c r="N109" s="6" t="s">
         <v>639</v>
-      </c>
-      <c r="H109" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="I109" s="6" t="s">
-        <v>573</v>
-      </c>
-      <c r="J109" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="K109" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="L109" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="M109" t="s">
-        <v>644</v>
-      </c>
-      <c r="N109" s="6" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -9504,7 +9477,7 @@
         <v>574</v>
       </c>
       <c r="G110" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H110" t="s">
         <v>574</v>
@@ -9522,10 +9495,10 @@
         <v>574</v>
       </c>
       <c r="M110" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N110" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -9566,7 +9539,7 @@
         <v>574</v>
       </c>
       <c r="M111" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -9589,7 +9562,7 @@
         <v>574</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H112" t="s">
         <v>573</v>
@@ -9607,10 +9580,10 @@
         <v>574</v>
       </c>
       <c r="M112" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="N112" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -9651,10 +9624,10 @@
         <v>574</v>
       </c>
       <c r="M113" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N113" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
@@ -9677,7 +9650,7 @@
         <v>574</v>
       </c>
       <c r="G114" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H114" t="s">
         <v>573</v>
@@ -9695,10 +9668,10 @@
         <v>574</v>
       </c>
       <c r="M114" t="s">
-        <v>635</v>
+        <v>681</v>
       </c>
       <c r="N114" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -9721,7 +9694,7 @@
         <v>574</v>
       </c>
       <c r="G115" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H115" t="s">
         <v>583</v>
@@ -9739,7 +9712,7 @@
         <v>574</v>
       </c>
       <c r="M115" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -9780,10 +9753,10 @@
         <v>574</v>
       </c>
       <c r="M116" t="s">
-        <v>735</v>
+        <v>693</v>
       </c>
       <c r="N116" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -9824,7 +9797,7 @@
         <v>574</v>
       </c>
       <c r="M117" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
@@ -9847,28 +9820,28 @@
         <v>574</v>
       </c>
       <c r="G118" t="s">
+        <v>648</v>
+      </c>
+      <c r="H118" t="s">
+        <v>574</v>
+      </c>
+      <c r="I118" t="s">
+        <v>574</v>
+      </c>
+      <c r="J118" t="s">
+        <v>574</v>
+      </c>
+      <c r="K118" t="s">
+        <v>574</v>
+      </c>
+      <c r="L118" t="s">
+        <v>574</v>
+      </c>
+      <c r="M118" t="s">
+        <v>643</v>
+      </c>
+      <c r="N118" t="s">
         <v>649</v>
-      </c>
-      <c r="H118" t="s">
-        <v>574</v>
-      </c>
-      <c r="I118" t="s">
-        <v>574</v>
-      </c>
-      <c r="J118" t="s">
-        <v>574</v>
-      </c>
-      <c r="K118" t="s">
-        <v>574</v>
-      </c>
-      <c r="L118" t="s">
-        <v>574</v>
-      </c>
-      <c r="M118" t="s">
-        <v>644</v>
-      </c>
-      <c r="N118" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
@@ -9909,7 +9882,7 @@
         <v>574</v>
       </c>
       <c r="M119" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
@@ -9932,7 +9905,7 @@
         <v>574</v>
       </c>
       <c r="G120" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="H120" t="s">
         <v>573</v>
@@ -9950,7 +9923,7 @@
         <v>574</v>
       </c>
       <c r="M120" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
@@ -9991,10 +9964,10 @@
         <v>574</v>
       </c>
       <c r="M121" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N121" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
@@ -10035,7 +10008,7 @@
         <v>574</v>
       </c>
       <c r="M122" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
@@ -10076,7 +10049,7 @@
         <v>574</v>
       </c>
       <c r="M123" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
@@ -10117,7 +10090,7 @@
         <v>574</v>
       </c>
       <c r="M124" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
@@ -10158,10 +10131,10 @@
         <v>574</v>
       </c>
       <c r="M125" t="s">
+        <v>652</v>
+      </c>
+      <c r="N125" t="s">
         <v>653</v>
-      </c>
-      <c r="N125" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
@@ -10184,28 +10157,28 @@
         <v>574</v>
       </c>
       <c r="G126" t="s">
+        <v>654</v>
+      </c>
+      <c r="H126" t="s">
+        <v>573</v>
+      </c>
+      <c r="I126" t="s">
+        <v>573</v>
+      </c>
+      <c r="J126" t="s">
+        <v>574</v>
+      </c>
+      <c r="K126" t="s">
+        <v>573</v>
+      </c>
+      <c r="L126" t="s">
+        <v>574</v>
+      </c>
+      <c r="M126" t="s">
+        <v>681</v>
+      </c>
+      <c r="N126" t="s">
         <v>655</v>
-      </c>
-      <c r="H126" t="s">
-        <v>573</v>
-      </c>
-      <c r="I126" t="s">
-        <v>573</v>
-      </c>
-      <c r="J126" t="s">
-        <v>574</v>
-      </c>
-      <c r="K126" t="s">
-        <v>573</v>
-      </c>
-      <c r="L126" t="s">
-        <v>574</v>
-      </c>
-      <c r="M126" t="s">
-        <v>682</v>
-      </c>
-      <c r="N126" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
@@ -10246,7 +10219,7 @@
         <v>574</v>
       </c>
       <c r="M127" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
@@ -10287,7 +10260,7 @@
         <v>574</v>
       </c>
       <c r="M128" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
@@ -10328,10 +10301,10 @@
         <v>574</v>
       </c>
       <c r="M129" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N129" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
@@ -10372,10 +10345,10 @@
         <v>574</v>
       </c>
       <c r="M130" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N130" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
@@ -10416,7 +10389,7 @@
         <v>574</v>
       </c>
       <c r="M131" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
@@ -10457,10 +10430,10 @@
         <v>574</v>
       </c>
       <c r="M132" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N132" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
@@ -10501,10 +10474,10 @@
         <v>574</v>
       </c>
       <c r="M133" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N133" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
@@ -10545,7 +10518,7 @@
         <v>574</v>
       </c>
       <c r="M134" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
@@ -10586,10 +10559,10 @@
         <v>574</v>
       </c>
       <c r="M135" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N135" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
@@ -10630,7 +10603,7 @@
         <v>574</v>
       </c>
       <c r="M136" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
@@ -10671,10 +10644,10 @@
         <v>574</v>
       </c>
       <c r="M137" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N137" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
@@ -10712,13 +10685,13 @@
         <v>573</v>
       </c>
       <c r="L138" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="M138" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N138" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
@@ -10759,7 +10732,7 @@
         <v>574</v>
       </c>
       <c r="M139" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
@@ -10782,28 +10755,28 @@
         <v>574</v>
       </c>
       <c r="G140" s="6" t="s">
+        <v>662</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="I140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="J140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="K140" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="L140" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="M140" t="s">
+        <v>693</v>
+      </c>
+      <c r="N140" s="6" t="s">
         <v>663</v>
-      </c>
-      <c r="H140" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="I140" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="J140" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="K140" s="6" t="s">
-        <v>573</v>
-      </c>
-      <c r="L140" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="M140" t="s">
-        <v>694</v>
-      </c>
-      <c r="N140" s="6" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
@@ -10844,7 +10817,7 @@
         <v>574</v>
       </c>
       <c r="M141" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
@@ -10885,7 +10858,7 @@
         <v>574</v>
       </c>
       <c r="M142" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
@@ -10926,10 +10899,10 @@
         <v>574</v>
       </c>
       <c r="M143" t="s">
-        <v>635</v>
+        <v>681</v>
       </c>
       <c r="N143" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
@@ -10952,7 +10925,7 @@
         <v>574</v>
       </c>
       <c r="G144" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H144" t="s">
         <v>573</v>
@@ -10970,7 +10943,7 @@
         <v>574</v>
       </c>
       <c r="M144" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
@@ -11011,10 +10984,10 @@
         <v>574</v>
       </c>
       <c r="M145" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N145" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
@@ -11055,10 +11028,10 @@
         <v>574</v>
       </c>
       <c r="M146" t="s">
-        <v>635</v>
+        <v>681</v>
       </c>
       <c r="N146" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
@@ -11099,10 +11072,10 @@
         <v>574</v>
       </c>
       <c r="M147" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N147" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
@@ -11143,10 +11116,10 @@
         <v>574</v>
       </c>
       <c r="M148" t="s">
-        <v>635</v>
+        <v>681</v>
       </c>
       <c r="N148" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
@@ -11187,7 +11160,7 @@
         <v>574</v>
       </c>
       <c r="M149" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
@@ -11228,10 +11201,10 @@
         <v>574</v>
       </c>
       <c r="M150" t="s">
-        <v>635</v>
+        <v>681</v>
       </c>
       <c r="N150" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
@@ -11272,10 +11245,10 @@
         <v>574</v>
       </c>
       <c r="M151" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N151" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
@@ -11316,10 +11289,10 @@
         <v>574</v>
       </c>
       <c r="M152" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N152" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
@@ -11360,7 +11333,7 @@
         <v>574</v>
       </c>
       <c r="M153" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
@@ -11401,10 +11374,10 @@
         <v>574</v>
       </c>
       <c r="M154" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N154" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
@@ -11445,7 +11418,7 @@
         <v>574</v>
       </c>
       <c r="M155" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
@@ -11486,10 +11459,10 @@
         <v>574</v>
       </c>
       <c r="M156" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N156" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
@@ -11530,10 +11503,10 @@
         <v>574</v>
       </c>
       <c r="M157" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N157" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
@@ -11556,28 +11529,28 @@
         <v>574</v>
       </c>
       <c r="G158" t="s">
+        <v>671</v>
+      </c>
+      <c r="H158" t="s">
+        <v>573</v>
+      </c>
+      <c r="I158" t="s">
+        <v>573</v>
+      </c>
+      <c r="J158" t="s">
+        <v>574</v>
+      </c>
+      <c r="K158" t="s">
+        <v>573</v>
+      </c>
+      <c r="L158" t="s">
+        <v>574</v>
+      </c>
+      <c r="M158" t="s">
+        <v>681</v>
+      </c>
+      <c r="N158" t="s">
         <v>672</v>
-      </c>
-      <c r="H158" t="s">
-        <v>573</v>
-      </c>
-      <c r="I158" t="s">
-        <v>573</v>
-      </c>
-      <c r="J158" t="s">
-        <v>574</v>
-      </c>
-      <c r="K158" t="s">
-        <v>573</v>
-      </c>
-      <c r="L158" t="s">
-        <v>574</v>
-      </c>
-      <c r="M158" t="s">
-        <v>682</v>
-      </c>
-      <c r="N158" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
@@ -11618,10 +11591,10 @@
         <v>574</v>
       </c>
       <c r="M159" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N159" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
@@ -11662,10 +11635,10 @@
         <v>574</v>
       </c>
       <c r="M160" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N160" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.2">
@@ -11706,10 +11679,10 @@
         <v>574</v>
       </c>
       <c r="M161" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N161" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
@@ -11750,10 +11723,10 @@
         <v>574</v>
       </c>
       <c r="M162" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N162" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.2">
@@ -11794,10 +11767,10 @@
         <v>574</v>
       </c>
       <c r="M163" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N163" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
@@ -11838,10 +11811,10 @@
         <v>574</v>
       </c>
       <c r="M164" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N164" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.2">
@@ -11882,7 +11855,7 @@
         <v>574</v>
       </c>
       <c r="M165" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
@@ -11923,7 +11896,7 @@
         <v>574</v>
       </c>
       <c r="M166" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.2">
@@ -11964,10 +11937,10 @@
         <v>574</v>
       </c>
       <c r="M167" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N167" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.2">
@@ -12008,10 +11981,10 @@
         <v>573</v>
       </c>
       <c r="M168" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="N168" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.2">
@@ -12034,7 +12007,7 @@
         <v>574</v>
       </c>
       <c r="G169" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H169" t="s">
         <v>573</v>
@@ -12093,10 +12066,10 @@
         <v>574</v>
       </c>
       <c r="M170" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="N170" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.2">
@@ -12119,28 +12092,28 @@
         <v>574</v>
       </c>
       <c r="G171" t="s">
+        <v>682</v>
+      </c>
+      <c r="H171" t="s">
+        <v>573</v>
+      </c>
+      <c r="I171" t="s">
+        <v>573</v>
+      </c>
+      <c r="J171" t="s">
+        <v>574</v>
+      </c>
+      <c r="K171" t="s">
+        <v>573</v>
+      </c>
+      <c r="L171" t="s">
+        <v>574</v>
+      </c>
+      <c r="M171" t="s">
         <v>683</v>
       </c>
-      <c r="H171" t="s">
-        <v>573</v>
-      </c>
-      <c r="I171" t="s">
-        <v>573</v>
-      </c>
-      <c r="J171" t="s">
-        <v>574</v>
-      </c>
-      <c r="K171" t="s">
-        <v>573</v>
-      </c>
-      <c r="L171" t="s">
-        <v>574</v>
-      </c>
-      <c r="M171" t="s">
-        <v>684</v>
-      </c>
       <c r="N171" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.2">
@@ -12181,7 +12154,7 @@
         <v>574</v>
       </c>
       <c r="M172" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.2">
@@ -12427,7 +12400,7 @@
         <v>574</v>
       </c>
       <c r="M178" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.2">
@@ -12468,10 +12441,10 @@
         <v>574</v>
       </c>
       <c r="M179" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N179" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.2">
@@ -12512,10 +12485,10 @@
         <v>574</v>
       </c>
       <c r="M180" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N180" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.2">
@@ -12556,10 +12529,10 @@
         <v>574</v>
       </c>
       <c r="M181" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N181" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.2">
@@ -12600,10 +12573,10 @@
         <v>574</v>
       </c>
       <c r="M182" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N182" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.2">
@@ -12644,10 +12617,10 @@
         <v>574</v>
       </c>
       <c r="M183" t="s">
+        <v>689</v>
+      </c>
+      <c r="N183" t="s">
         <v>690</v>
-      </c>
-      <c r="N183" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.2">
@@ -12688,10 +12661,10 @@
         <v>574</v>
       </c>
       <c r="M184" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N184" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.2">
@@ -12735,7 +12708,7 @@
         <v>615</v>
       </c>
       <c r="N185" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.2">
@@ -12776,10 +12749,10 @@
         <v>574</v>
       </c>
       <c r="M186" t="s">
+        <v>693</v>
+      </c>
+      <c r="N186" t="s">
         <v>694</v>
-      </c>
-      <c r="N186" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.2">
@@ -12861,10 +12834,10 @@
         <v>574</v>
       </c>
       <c r="M188" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N188" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.2">
@@ -12905,10 +12878,10 @@
         <v>573</v>
       </c>
       <c r="M189" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N189" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.2">
@@ -12949,10 +12922,10 @@
         <v>574</v>
       </c>
       <c r="M190" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N190" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.2">
@@ -12993,10 +12966,10 @@
         <v>574</v>
       </c>
       <c r="M191" s="6" t="s">
+        <v>697</v>
+      </c>
+      <c r="N191" s="6" t="s">
         <v>698</v>
-      </c>
-      <c r="N191" s="6" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.2">
@@ -13119,10 +13092,10 @@
         <v>574</v>
       </c>
       <c r="M194" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N194" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.2">
@@ -13163,10 +13136,10 @@
         <v>574</v>
       </c>
       <c r="M195" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N195" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.2">
@@ -13207,10 +13180,10 @@
         <v>574</v>
       </c>
       <c r="M196" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N196" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.2">
@@ -13251,10 +13224,10 @@
         <v>574</v>
       </c>
       <c r="M197" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N197" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.2">
@@ -13295,10 +13268,10 @@
         <v>574</v>
       </c>
       <c r="M198" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N198" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.2">
@@ -13339,7 +13312,7 @@
         <v>574</v>
       </c>
       <c r="M199" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.2">
@@ -13380,7 +13353,7 @@
         <v>574</v>
       </c>
       <c r="M200" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.2">
@@ -13421,10 +13394,10 @@
         <v>574</v>
       </c>
       <c r="M201" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N201" s="6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.2">
@@ -13447,7 +13420,7 @@
         <v>574</v>
       </c>
       <c r="G202" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H202" t="s">
         <v>583</v>
@@ -13488,7 +13461,7 @@
         <v>574</v>
       </c>
       <c r="G203" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H203" t="s">
         <v>583</v>
@@ -13588,10 +13561,10 @@
         <v>574</v>
       </c>
       <c r="M205" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N205" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.2">
@@ -13673,10 +13646,10 @@
         <v>574</v>
       </c>
       <c r="M207" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N207" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.2">
@@ -13802,7 +13775,7 @@
         <v>615</v>
       </c>
       <c r="N210" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.2">
@@ -13887,7 +13860,7 @@
         <v>615</v>
       </c>
       <c r="N212" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.2">
@@ -14033,7 +14006,7 @@
         <v>574</v>
       </c>
       <c r="G216" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H216" t="s">
         <v>574</v>
@@ -14133,10 +14106,10 @@
         <v>574</v>
       </c>
       <c r="M218" s="6" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N218" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.2">
@@ -14282,7 +14255,7 @@
         <v>574</v>
       </c>
       <c r="G222" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H222" t="s">
         <v>573</v>
@@ -14341,10 +14314,10 @@
         <v>574</v>
       </c>
       <c r="M223" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N223" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.2">
@@ -14552,7 +14525,7 @@
         <v>619</v>
       </c>
       <c r="N228" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.2">
@@ -14575,7 +14548,7 @@
         <v>574</v>
       </c>
       <c r="G229" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H229" t="s">
         <v>574</v>
@@ -14593,10 +14566,10 @@
         <v>574</v>
       </c>
       <c r="M229" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N229" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.2">
@@ -15088,10 +15061,10 @@
         <v>574</v>
       </c>
       <c r="M241" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N241" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="242" spans="1:14" x14ac:dyDescent="0.2">
@@ -15114,7 +15087,7 @@
         <v>574</v>
       </c>
       <c r="G242" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H242" t="s">
         <v>583</v>
@@ -15132,10 +15105,10 @@
         <v>574</v>
       </c>
       <c r="M242" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N242" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.2">
@@ -15176,7 +15149,7 @@
         <v>574</v>
       </c>
       <c r="M243" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="244" spans="1:14" x14ac:dyDescent="0.2">
@@ -15217,7 +15190,7 @@
         <v>574</v>
       </c>
       <c r="M244" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="245" spans="1:14" x14ac:dyDescent="0.2">
@@ -15258,7 +15231,7 @@
         <v>574</v>
       </c>
       <c r="M245" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.2">
@@ -15281,7 +15254,7 @@
         <v>574</v>
       </c>
       <c r="G246" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H246" t="s">
         <v>574</v>
@@ -15299,7 +15272,7 @@
         <v>574</v>
       </c>
       <c r="M246" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="247" spans="1:14" x14ac:dyDescent="0.2">
@@ -15463,10 +15436,10 @@
         <v>574</v>
       </c>
       <c r="M250" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N250" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="251" spans="1:14" x14ac:dyDescent="0.2">
@@ -15589,7 +15562,7 @@
         <v>573</v>
       </c>
       <c r="M253" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N253" t="s">
         <v>604</v>
@@ -15677,7 +15650,7 @@
         <v>592</v>
       </c>
       <c r="N255" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.2">
@@ -15759,10 +15732,10 @@
         <v>574</v>
       </c>
       <c r="M257" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="N257" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.2">
@@ -15885,10 +15858,10 @@
         <v>574</v>
       </c>
       <c r="M260" t="s">
+        <v>716</v>
+      </c>
+      <c r="N260" t="s">
         <v>717</v>
-      </c>
-      <c r="N260" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="261" spans="1:14" x14ac:dyDescent="0.2">
@@ -15993,7 +15966,7 @@
         <v>574</v>
       </c>
       <c r="G263" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H263" t="s">
         <v>573</v>
@@ -16198,7 +16171,7 @@
         <v>574</v>
       </c>
       <c r="G268" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H268" t="s">
         <v>573</v>
@@ -16257,10 +16230,10 @@
         <v>574</v>
       </c>
       <c r="M269" t="s">
+        <v>719</v>
+      </c>
+      <c r="N269" t="s">
         <v>720</v>
-      </c>
-      <c r="N269" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="270" spans="1:14" x14ac:dyDescent="0.2">
@@ -16301,7 +16274,7 @@
         <v>574</v>
       </c>
       <c r="M270" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="271" spans="1:14" x14ac:dyDescent="0.2">
@@ -16324,7 +16297,7 @@
         <v>574</v>
       </c>
       <c r="G271" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H271" t="s">
         <v>573</v>
@@ -16547,10 +16520,10 @@
         <v>574</v>
       </c>
       <c r="M276" t="s">
+        <v>719</v>
+      </c>
+      <c r="N276" t="s">
         <v>720</v>
-      </c>
-      <c r="N276" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="277" spans="1:14" x14ac:dyDescent="0.2">
@@ -16714,7 +16687,7 @@
         <v>574</v>
       </c>
       <c r="M280" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="281" spans="1:14" x14ac:dyDescent="0.2">
@@ -16755,7 +16728,7 @@
         <v>574</v>
       </c>
       <c r="M281" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.2">
@@ -16837,10 +16810,10 @@
         <v>574</v>
       </c>
       <c r="M283" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N283" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.2">
@@ -17557,7 +17530,7 @@
         <v>266</v>
       </c>
       <c r="F301" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G301" t="s">
         <v>574</v>
@@ -17578,10 +17551,10 @@
         <v>574</v>
       </c>
       <c r="M301" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="N301" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to excel file
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B31678B-D4A6-EB41-A64B-0076A7F8201D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36444796-692F-7047-8701-D58702DA1238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="760" windowWidth="26140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34460" yWindow="1000" windowWidth="26140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="734">
   <si>
     <t>type</t>
   </si>
@@ -4318,9 +4318,6 @@
   </si>
   <si>
     <t>abstract is longer in the metadata; XML shows update after initial deposit</t>
-  </si>
-  <si>
-    <t>"en</t>
   </si>
   <si>
     <t>includes HTML</t>
@@ -4769,10 +4766,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L150" sqref="L150"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4822,7 +4819,7 @@
         <v>598</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>570</v>
@@ -4848,7 +4845,7 @@
         <v>10871</v>
       </c>
       <c r="F2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G2" t="s">
         <v>574</v>
@@ -4869,7 +4866,7 @@
         <v>574</v>
       </c>
       <c r="M2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -4910,7 +4907,7 @@
         <v>574</v>
       </c>
       <c r="M3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -5036,10 +5033,10 @@
         <v>574</v>
       </c>
       <c r="M6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -5144,7 +5141,7 @@
         <v>6937</v>
       </c>
       <c r="F9" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G9" t="s">
         <v>574</v>
@@ -5165,7 +5162,7 @@
         <v>574</v>
       </c>
       <c r="M9" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="N9" t="s">
         <v>578</v>
@@ -5188,10 +5185,10 @@
         <v>6602</v>
       </c>
       <c r="F10" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G10" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
       <c r="H10" t="s">
         <v>573</v>
@@ -5209,7 +5206,7 @@
         <v>574</v>
       </c>
       <c r="M10" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -5229,7 +5226,7 @@
         <v>6576</v>
       </c>
       <c r="F11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G11" t="s">
         <v>574</v>
@@ -5250,7 +5247,7 @@
         <v>573</v>
       </c>
       <c r="M11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N11" t="s">
         <v>579</v>
@@ -5294,7 +5291,7 @@
         <v>573</v>
       </c>
       <c r="M12" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N12" t="s">
         <v>582</v>
@@ -5382,7 +5379,7 @@
         <v>573</v>
       </c>
       <c r="M14" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N14" t="s">
         <v>581</v>
@@ -5446,7 +5443,7 @@
         <v>5878</v>
       </c>
       <c r="F16" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G16" t="s">
         <v>574</v>
@@ -5467,7 +5464,7 @@
         <v>573</v>
       </c>
       <c r="M16" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N16" t="s">
         <v>584</v>
@@ -5534,7 +5531,7 @@
         <v>5526</v>
       </c>
       <c r="F18" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G18" t="s">
         <v>574</v>
@@ -5599,7 +5596,7 @@
         <v>574</v>
       </c>
       <c r="M19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N19" t="s">
         <v>587</v>
@@ -5622,7 +5619,7 @@
         <v>5490</v>
       </c>
       <c r="F20" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G20" t="s">
         <v>574</v>
@@ -5643,7 +5640,7 @@
         <v>574</v>
       </c>
       <c r="M20" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -5684,7 +5681,7 @@
         <v>573</v>
       </c>
       <c r="M21" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N21" t="s">
         <v>588</v>
@@ -5728,7 +5725,7 @@
         <v>573</v>
       </c>
       <c r="M22" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="N22" t="s">
         <v>580</v>
@@ -5751,7 +5748,7 @@
         <v>5272</v>
       </c>
       <c r="F23" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G23" t="s">
         <v>574</v>
@@ -5772,7 +5769,7 @@
         <v>574</v>
       </c>
       <c r="M23" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N23" t="s">
         <v>589</v>
@@ -5795,7 +5792,7 @@
         <v>5209</v>
       </c>
       <c r="F24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G24" t="s">
         <v>574</v>
@@ -5883,7 +5880,7 @@
         <v>5162</v>
       </c>
       <c r="F26" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G26" t="s">
         <v>574</v>
@@ -5904,7 +5901,7 @@
         <v>573</v>
       </c>
       <c r="M26" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N26" t="s">
         <v>580</v>
@@ -6206,7 +6203,7 @@
         <v>573</v>
       </c>
       <c r="M33" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N33" t="s">
         <v>600</v>
@@ -6291,7 +6288,7 @@
         <v>573</v>
       </c>
       <c r="M35" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N35" t="s">
         <v>604</v>
@@ -6335,7 +6332,7 @@
         <v>573</v>
       </c>
       <c r="M36" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N36" t="s">
         <v>604</v>
@@ -6379,7 +6376,7 @@
         <v>573</v>
       </c>
       <c r="M37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N37" t="s">
         <v>604</v>
@@ -6508,7 +6505,7 @@
         <v>573</v>
       </c>
       <c r="M40" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N40" t="s">
         <v>606</v>
@@ -6552,7 +6549,7 @@
         <v>573</v>
       </c>
       <c r="M41" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N41" t="s">
         <v>607</v>
@@ -6596,7 +6593,7 @@
         <v>573</v>
       </c>
       <c r="M42" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N42" t="s">
         <v>608</v>
@@ -6722,7 +6719,7 @@
         <v>573</v>
       </c>
       <c r="M45" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N45" t="s">
         <v>604</v>
@@ -6766,7 +6763,7 @@
         <v>574</v>
       </c>
       <c r="M46" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -7068,7 +7065,7 @@
         <v>573</v>
       </c>
       <c r="M53" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N53" t="s">
         <v>613</v>
@@ -7112,7 +7109,7 @@
         <v>573</v>
       </c>
       <c r="M54" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N54" t="s">
         <v>613</v>
@@ -7156,7 +7153,7 @@
         <v>573</v>
       </c>
       <c r="M55" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="N55" t="s">
         <v>612</v>
@@ -7200,7 +7197,7 @@
         <v>573</v>
       </c>
       <c r="M56" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="N56" t="s">
         <v>614</v>
@@ -7244,7 +7241,7 @@
         <v>573</v>
       </c>
       <c r="M57" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N57" t="s">
         <v>604</v>
@@ -7560,7 +7557,7 @@
         <v>4362</v>
       </c>
       <c r="F65" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G65" t="s">
         <v>574</v>
@@ -7581,7 +7578,7 @@
         <v>574</v>
       </c>
       <c r="M65" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -7704,7 +7701,7 @@
         <v>574</v>
       </c>
       <c r="M68" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N68" t="s">
         <v>621</v>
@@ -7748,7 +7745,7 @@
         <v>574</v>
       </c>
       <c r="M69" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -7833,7 +7830,7 @@
         <v>574</v>
       </c>
       <c r="M71" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N71" t="s">
         <v>623</v>
@@ -7877,7 +7874,7 @@
         <v>573</v>
       </c>
       <c r="M72" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N72" t="s">
         <v>604</v>
@@ -7921,7 +7918,7 @@
         <v>573</v>
       </c>
       <c r="M73" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N73" t="s">
         <v>624</v>
@@ -7965,7 +7962,7 @@
         <v>574</v>
       </c>
       <c r="M74" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -8006,7 +8003,7 @@
         <v>574</v>
       </c>
       <c r="M75" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N75" t="s">
         <v>623</v>
@@ -8029,7 +8026,7 @@
         <v>4185</v>
       </c>
       <c r="F76" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G76" t="s">
         <v>574</v>
@@ -8138,7 +8135,7 @@
         <v>574</v>
       </c>
       <c r="M78" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N78" t="s">
         <v>628</v>
@@ -8182,7 +8179,7 @@
         <v>574</v>
       </c>
       <c r="M79" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -8202,7 +8199,7 @@
         <v>4162</v>
       </c>
       <c r="F80" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G80" t="s">
         <v>601</v>
@@ -8223,7 +8220,7 @@
         <v>574</v>
       </c>
       <c r="M80" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -8428,7 +8425,7 @@
         <v>574</v>
       </c>
       <c r="M85" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -8448,7 +8445,7 @@
         <v>4100</v>
       </c>
       <c r="F86" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G86" t="s">
         <v>574</v>
@@ -8513,7 +8510,7 @@
         <v>574</v>
       </c>
       <c r="M87" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N87" t="s">
         <v>630</v>
@@ -8642,7 +8639,7 @@
         <v>574</v>
       </c>
       <c r="M90" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N90" t="s">
         <v>632</v>
@@ -8706,7 +8703,7 @@
         <v>4045</v>
       </c>
       <c r="F92" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G92" t="s">
         <v>601</v>
@@ -8982,7 +8979,7 @@
         <v>574</v>
       </c>
       <c r="M98" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N98" t="s">
         <v>633</v>
@@ -9108,7 +9105,7 @@
         <v>574</v>
       </c>
       <c r="M101" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="N101" t="s">
         <v>634</v>
@@ -12834,7 +12831,7 @@
         <v>574</v>
       </c>
       <c r="M188" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N188" t="s">
         <v>695</v>
@@ -15436,7 +15433,7 @@
         <v>574</v>
       </c>
       <c r="M250" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N250" t="s">
         <v>713</v>
@@ -16171,7 +16168,7 @@
         <v>574</v>
       </c>
       <c r="G268" t="s">
-        <v>718</v>
+        <v>601</v>
       </c>
       <c r="H268" t="s">
         <v>573</v>
@@ -16230,10 +16227,10 @@
         <v>574</v>
       </c>
       <c r="M269" t="s">
+        <v>718</v>
+      </c>
+      <c r="N269" t="s">
         <v>719</v>
-      </c>
-      <c r="N269" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="270" spans="1:14" x14ac:dyDescent="0.2">
@@ -16520,10 +16517,10 @@
         <v>574</v>
       </c>
       <c r="M276" t="s">
+        <v>718</v>
+      </c>
+      <c r="N276" t="s">
         <v>719</v>
-      </c>
-      <c r="N276" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="277" spans="1:14" x14ac:dyDescent="0.2">
@@ -16687,7 +16684,7 @@
         <v>574</v>
       </c>
       <c r="M280" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="281" spans="1:14" x14ac:dyDescent="0.2">
@@ -16728,7 +16725,7 @@
         <v>574</v>
       </c>
       <c r="M281" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.2">
@@ -16810,10 +16807,10 @@
         <v>574</v>
       </c>
       <c r="M283" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N283" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.2">
@@ -17530,7 +17527,7 @@
         <v>266</v>
       </c>
       <c r="F301" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G301" t="s">
         <v>574</v>
@@ -17551,10 +17548,10 @@
         <v>574</v>
       </c>
       <c r="M301" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="N301" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small update to part 1
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5214CF02-0346-4C4B-9345-8B80021FFC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CFF3EB-0266-E748-AF75-A910DD8E2608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="26140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="760" windowWidth="27980" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4764,13 +4764,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C106" sqref="C106"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4783,7 +4782,8 @@
     <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="37.1640625" customWidth="1"/>
     <col min="14" max="14" width="75" bestFit="1" customWidth="1"/>
   </cols>
@@ -4829,7 +4829,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="23" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -6339,7 +6339,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -6556,7 +6556,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8265,7 +8265,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8517,7 +8517,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8602,7 +8602,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -8775,7 +8775,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -8986,7 +8986,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -9027,7 +9027,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -9068,7 +9068,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -9156,7 +9156,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -9672,7 +9672,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -9798,7 +9798,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -9924,7 +9924,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -10009,7 +10009,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -10434,7 +10434,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -10733,7 +10733,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
         <v>138</v>
       </c>
@@ -10944,7 +10944,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -11205,7 +11205,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -11249,7 +11249,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -11463,7 +11463,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -11639,7 +11639,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
         <v>159</v>
       </c>
@@ -11856,7 +11856,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -11897,7 +11897,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -11941,7 +11941,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -12026,7 +12026,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -12070,7 +12070,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -12196,7 +12196,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -12237,7 +12237,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -12278,7 +12278,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -12577,7 +12577,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -12665,7 +12665,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -12709,7 +12709,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -12753,7 +12753,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="187" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -12794,7 +12794,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
         <v>189</v>
       </c>
@@ -12970,7 +12970,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -13011,7 +13011,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -13052,7 +13052,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -13140,7 +13140,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -13184,7 +13184,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -13272,7 +13272,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201" s="7">
         <v>199</v>
       </c>
@@ -13398,7 +13398,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -13439,7 +13439,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -13480,7 +13480,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -13521,7 +13521,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -13565,7 +13565,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -13650,7 +13650,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -13691,7 +13691,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -13732,7 +13732,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -13776,7 +13776,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -13861,7 +13861,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -13902,7 +13902,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -13984,7 +13984,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -14025,7 +14025,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -14066,7 +14066,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218" s="7">
         <v>216</v>
       </c>
@@ -14110,7 +14110,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -14151,7 +14151,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -14192,7 +14192,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -14233,7 +14233,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -14274,7 +14274,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -14318,7 +14318,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -14359,7 +14359,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -14400,7 +14400,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -14441,7 +14441,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -14482,7 +14482,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -14526,7 +14526,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -14570,7 +14570,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -14652,7 +14652,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -14693,7 +14693,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -14734,7 +14734,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -14857,7 +14857,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -14898,7 +14898,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -14939,7 +14939,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -14980,7 +14980,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -15021,7 +15021,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -15065,7 +15065,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -15109,7 +15109,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -15232,7 +15232,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -15273,7 +15273,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -15314,7 +15314,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -15355,7 +15355,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -15396,7 +15396,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -15440,7 +15440,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -15481,7 +15481,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -15522,7 +15522,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -15566,7 +15566,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -15607,7 +15607,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -15651,7 +15651,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -15692,7 +15692,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="257" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -15736,7 +15736,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="258" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -15777,7 +15777,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="259" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -15818,7 +15818,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="260" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -15862,7 +15862,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="261" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -15903,7 +15903,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="262" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -15944,7 +15944,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="263" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -15985,7 +15985,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="264" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -16026,7 +16026,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="265" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -16067,7 +16067,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="266" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -16108,7 +16108,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="267" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -16149,7 +16149,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="268" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -16190,7 +16190,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="269" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -16234,7 +16234,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="270" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -16275,7 +16275,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="271" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -16316,7 +16316,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="272" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -16357,7 +16357,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="273" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -16398,7 +16398,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="274" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -16439,7 +16439,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="275" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -16480,7 +16480,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="276" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -16524,7 +16524,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="277" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -16565,7 +16565,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="278" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -16606,7 +16606,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="279" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -16647,7 +16647,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="280" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -16688,7 +16688,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="281" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -16729,7 +16729,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="282" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -16770,7 +16770,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="283" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -16814,7 +16814,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="284" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -16855,7 +16855,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="285" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -16896,7 +16896,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="286" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -16937,7 +16937,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="287" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -16978,7 +16978,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="288" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -17019,7 +17019,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="289" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -17060,7 +17060,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="290" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -17101,7 +17101,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="291" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -17142,7 +17142,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="292" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -17183,7 +17183,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="293" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -17224,7 +17224,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="294" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -17265,7 +17265,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="295" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -17306,7 +17306,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="296" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -17347,7 +17347,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="297" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -17388,7 +17388,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="298" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -17429,7 +17429,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="299" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -17470,7 +17470,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -17511,7 +17511,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -17556,13 +17556,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N301" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="no abstract in article"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N301" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
such good work today! Part 1 is done with analysis
</commit_message>
<xml_diff>
--- a/data/part_1_df_abstract_subset.xlsx
+++ b/data/part_1_df_abstract_subset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DF1118-D0AA-9945-AF13-D55D08CA29CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47AA9D7-08B7-AD44-B418-9D31762C5188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="27980" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="780" windowWidth="27980" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>